<commit_message>
Update simulations diary file
</commit_message>
<xml_diff>
--- a/simulationsDiary.xlsx
+++ b/simulationsDiary.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="17426"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ETH\code\abaqus\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="480" yWindow="120" windowWidth="19980" windowHeight="6810"/>
   </bookViews>
@@ -16,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="71">
   <si>
     <t>typeOfModel</t>
   </si>
@@ -221,11 +226,20 @@
   <si>
     <t>Try with inner ribs</t>
   </si>
+  <si>
+    <t>Decrease a bit the load to see convergence</t>
+  </si>
+  <si>
+    <t>Converged. The rib at the tip it's losing its in plane shape.</t>
+  </si>
+  <si>
+    <t>Good result. Still little deformation</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -293,13 +307,16 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:Z30" totalsRowShown="0">
-  <autoFilter ref="A1:Z30"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:Z33" totalsRowShown="0">
+  <autoFilter ref="A1:Z33"/>
   <tableColumns count="26">
     <tableColumn id="1" name="typeOfModel"/>
     <tableColumn id="2" name="Erib/E1"/>
@@ -375,7 +392,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -408,9 +425,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -443,6 +477,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -619,10 +670,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:BK314"/>
+  <dimension ref="A1:BK317"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="V20" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AA27" sqref="AA27"/>
+    <sheetView tabSelected="1" topLeftCell="A26" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G31" sqref="G31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3482,7 +3533,7 @@
         <v>10</v>
       </c>
       <c r="F27" s="2">
-        <v>0.8</v>
+        <v>1</v>
       </c>
       <c r="G27" s="2">
         <v>2</v>
@@ -3491,7 +3542,7 @@
         <v>2</v>
       </c>
       <c r="I27" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J27" s="2" t="s">
         <v>22</v>
@@ -3515,25 +3566,31 @@
         <v>36</v>
       </c>
       <c r="Q27" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="R27" s="2">
         <v>0.5</v>
       </c>
       <c r="S27" s="2">
-        <v>-1500</v>
+        <v>-1000</v>
       </c>
       <c r="T27" s="2">
         <v>20</v>
       </c>
       <c r="U27" s="2">
-        <v>3</v>
-      </c>
-      <c r="V27" s="4"/>
+        <v>2</v>
+      </c>
+      <c r="V27" s="2"/>
       <c r="W27" s="2"/>
-      <c r="X27" s="2"/>
-      <c r="Y27" s="2"/>
-      <c r="Z27" s="2"/>
+      <c r="X27" s="2">
+        <v>0.95</v>
+      </c>
+      <c r="Y27" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="Z27" s="2" t="s">
+        <v>68</v>
+      </c>
       <c r="AA27" s="2"/>
       <c r="AB27" s="2"/>
       <c r="AC27" s="2"/>
@@ -3587,7 +3644,7 @@
         <v>10</v>
       </c>
       <c r="F28" s="2">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="G28" s="2">
         <v>2</v>
@@ -3596,7 +3653,7 @@
         <v>2</v>
       </c>
       <c r="I28" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J28" s="2" t="s">
         <v>22</v>
@@ -3605,7 +3662,7 @@
         <v>22</v>
       </c>
       <c r="L28" s="2">
-        <v>40</v>
+        <v>25</v>
       </c>
       <c r="M28" s="2">
         <v>300</v>
@@ -3620,32 +3677,30 @@
         <v>36</v>
       </c>
       <c r="Q28" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="R28" s="2">
         <v>0.5</v>
       </c>
       <c r="S28" s="2">
-        <v>-500</v>
+        <v>-900</v>
       </c>
       <c r="T28" s="2">
         <v>20</v>
       </c>
       <c r="U28" s="2">
-        <v>3</v>
-      </c>
-      <c r="V28" s="4">
-        <v>-1.2799999999999999E-4</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="V28" s="2"/>
       <c r="W28" s="2"/>
       <c r="X28" s="2">
         <v>1</v>
       </c>
       <c r="Y28" s="2" t="s">
-        <v>45</v>
+        <v>69</v>
       </c>
       <c r="Z28" s="2" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="AA28" s="2"/>
       <c r="AB28" s="2"/>
@@ -3700,7 +3755,7 @@
         <v>10</v>
       </c>
       <c r="F29" s="2">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="G29" s="2">
         <v>2</v>
@@ -3709,7 +3764,7 @@
         <v>2</v>
       </c>
       <c r="I29" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J29" s="2" t="s">
         <v>22</v>
@@ -3733,27 +3788,27 @@
         <v>36</v>
       </c>
       <c r="Q29" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="R29" s="2">
         <v>0.5</v>
       </c>
       <c r="S29" s="2">
-        <v>-1000</v>
+        <v>-900</v>
       </c>
       <c r="T29" s="2">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="U29" s="2">
-        <v>3</v>
-      </c>
-      <c r="V29" s="4"/>
+        <v>2</v>
+      </c>
+      <c r="V29" s="2"/>
       <c r="W29" s="2"/>
       <c r="X29" s="2">
-        <v>0.87</v>
+        <v>1</v>
       </c>
       <c r="Y29" s="2" t="s">
-        <v>47</v>
+        <v>70</v>
       </c>
       <c r="Z29" s="2"/>
       <c r="AA29" s="2"/>
@@ -3792,32 +3847,73 @@
       <c r="BH29" s="2"/>
       <c r="BI29" s="2"/>
     </row>
-    <row r="30" spans="1:61" x14ac:dyDescent="0.25">
-      <c r="A30" s="2"/>
-      <c r="B30" s="2"/>
-      <c r="C30" s="2"/>
-      <c r="D30" s="2"/>
-      <c r="E30" s="2"/>
-      <c r="F30" s="2"/>
-      <c r="G30" s="2"/>
-      <c r="H30" s="2"/>
-      <c r="I30" s="2"/>
-      <c r="J30" s="2"/>
-      <c r="K30" s="2"/>
-      <c r="L30" s="2"/>
-      <c r="M30" s="2"/>
-      <c r="N30" s="2"/>
-      <c r="O30" s="2"/>
-      <c r="P30" s="2"/>
-      <c r="Q30" s="2"/>
-      <c r="R30" s="2"/>
-      <c r="S30" s="2"/>
-      <c r="T30" s="2"/>
-      <c r="U30" s="2"/>
-      <c r="V30" s="2"/>
+    <row r="30" spans="1:61" ht="30" x14ac:dyDescent="0.25">
+      <c r="A30" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B30" s="2">
+        <v>10</v>
+      </c>
+      <c r="C30" s="2">
+        <v>8</v>
+      </c>
+      <c r="D30" s="2">
+        <v>3</v>
+      </c>
+      <c r="E30" s="2">
+        <v>10</v>
+      </c>
+      <c r="F30" s="2">
+        <v>0.8</v>
+      </c>
+      <c r="G30" s="2">
+        <v>2</v>
+      </c>
+      <c r="H30" s="2">
+        <v>2</v>
+      </c>
+      <c r="I30" s="2">
+        <v>1</v>
+      </c>
+      <c r="J30" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="K30" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="L30" s="2">
+        <v>25</v>
+      </c>
+      <c r="M30" s="2">
+        <v>300</v>
+      </c>
+      <c r="N30" s="2">
+        <v>0.01</v>
+      </c>
+      <c r="O30" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="P30" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q30" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="R30" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="S30" s="2">
+        <v>-1500</v>
+      </c>
+      <c r="T30" s="2">
+        <v>30</v>
+      </c>
+      <c r="U30" s="2">
+        <v>4</v>
+      </c>
+      <c r="V30" s="4"/>
       <c r="W30" s="2"/>
       <c r="X30" s="2"/>
-      <c r="Y30" s="2"/>
       <c r="Z30" s="2"/>
       <c r="AA30" s="2"/>
       <c r="AB30" s="2"/>
@@ -3855,33 +3951,83 @@
       <c r="BH30" s="2"/>
       <c r="BI30" s="2"/>
     </row>
-    <row r="31" spans="1:61" x14ac:dyDescent="0.25">
-      <c r="A31" s="2"/>
-      <c r="B31" s="2"/>
-      <c r="C31" s="2"/>
-      <c r="D31" s="2"/>
-      <c r="E31" s="2"/>
-      <c r="F31" s="2"/>
-      <c r="G31" s="2"/>
-      <c r="H31" s="2"/>
-      <c r="I31" s="2"/>
-      <c r="J31" s="2"/>
-      <c r="K31" s="2"/>
-      <c r="L31" s="2"/>
-      <c r="M31" s="2"/>
-      <c r="N31" s="2"/>
-      <c r="O31" s="2"/>
-      <c r="P31" s="2"/>
-      <c r="Q31" s="2"/>
-      <c r="R31" s="2"/>
-      <c r="S31" s="2"/>
-      <c r="T31" s="2"/>
-      <c r="U31" s="2"/>
-      <c r="V31" s="2"/>
+    <row r="31" spans="1:61" ht="30" x14ac:dyDescent="0.25">
+      <c r="A31" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B31" s="2">
+        <v>10</v>
+      </c>
+      <c r="C31" s="2">
+        <v>8</v>
+      </c>
+      <c r="D31" s="2">
+        <v>3</v>
+      </c>
+      <c r="E31" s="2">
+        <v>10</v>
+      </c>
+      <c r="F31" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="G31" s="2">
+        <v>2</v>
+      </c>
+      <c r="H31" s="2">
+        <v>2</v>
+      </c>
+      <c r="I31" s="2">
+        <v>1</v>
+      </c>
+      <c r="J31" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="K31" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="L31" s="2">
+        <v>40</v>
+      </c>
+      <c r="M31" s="2">
+        <v>300</v>
+      </c>
+      <c r="N31" s="2">
+        <v>0.01</v>
+      </c>
+      <c r="O31" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="P31" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q31" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="R31" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="S31" s="2">
+        <v>-500</v>
+      </c>
+      <c r="T31" s="2">
+        <v>20</v>
+      </c>
+      <c r="U31" s="2">
+        <v>3</v>
+      </c>
+      <c r="V31" s="4">
+        <v>-1.2799999999999999E-4</v>
+      </c>
       <c r="W31" s="2"/>
-      <c r="X31" s="2"/>
-      <c r="Y31" s="2"/>
-      <c r="Z31" s="2"/>
+      <c r="X31" s="2">
+        <v>1</v>
+      </c>
+      <c r="Y31" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="Z31" s="2" t="s">
+        <v>46</v>
+      </c>
       <c r="AA31" s="2"/>
       <c r="AB31" s="2"/>
       <c r="AC31" s="2"/>
@@ -3918,32 +4064,78 @@
       <c r="BH31" s="2"/>
       <c r="BI31" s="2"/>
     </row>
-    <row r="32" spans="1:61" x14ac:dyDescent="0.25">
-      <c r="A32" s="2"/>
-      <c r="B32" s="2"/>
-      <c r="C32" s="2"/>
-      <c r="D32" s="2"/>
-      <c r="E32" s="2"/>
-      <c r="F32" s="2"/>
-      <c r="G32" s="2"/>
-      <c r="H32" s="2"/>
-      <c r="I32" s="2"/>
-      <c r="J32" s="2"/>
-      <c r="K32" s="2"/>
-      <c r="L32" s="2"/>
-      <c r="M32" s="2"/>
-      <c r="N32" s="2"/>
-      <c r="O32" s="2"/>
-      <c r="P32" s="2"/>
-      <c r="Q32" s="2"/>
-      <c r="R32" s="2"/>
-      <c r="S32" s="2"/>
-      <c r="T32" s="2"/>
-      <c r="U32" s="2"/>
-      <c r="V32" s="2"/>
+    <row r="32" spans="1:61" ht="30" x14ac:dyDescent="0.25">
+      <c r="A32" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B32" s="2">
+        <v>10</v>
+      </c>
+      <c r="C32" s="2">
+        <v>8</v>
+      </c>
+      <c r="D32" s="2">
+        <v>3</v>
+      </c>
+      <c r="E32" s="2">
+        <v>10</v>
+      </c>
+      <c r="F32" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="G32" s="2">
+        <v>2</v>
+      </c>
+      <c r="H32" s="2">
+        <v>2</v>
+      </c>
+      <c r="I32" s="2">
+        <v>1</v>
+      </c>
+      <c r="J32" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="K32" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="L32" s="2">
+        <v>40</v>
+      </c>
+      <c r="M32" s="2">
+        <v>300</v>
+      </c>
+      <c r="N32" s="2">
+        <v>0.01</v>
+      </c>
+      <c r="O32" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="P32" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q32" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="R32" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="S32" s="2">
+        <v>-1000</v>
+      </c>
+      <c r="T32" s="2">
+        <v>20</v>
+      </c>
+      <c r="U32" s="2">
+        <v>3</v>
+      </c>
+      <c r="V32" s="4"/>
       <c r="W32" s="2"/>
-      <c r="X32" s="2"/>
-      <c r="Y32" s="2"/>
+      <c r="X32" s="2">
+        <v>0.87</v>
+      </c>
+      <c r="Y32" s="2" t="s">
+        <v>47</v>
+      </c>
       <c r="Z32" s="2"/>
       <c r="AA32" s="2"/>
       <c r="AB32" s="2"/>
@@ -21017,6 +21209,7 @@
       <c r="W313" s="2"/>
       <c r="X313" s="2"/>
       <c r="Y313" s="2"/>
+      <c r="Z313" s="2"/>
     </row>
     <row r="314" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A314" s="2"/>
@@ -21043,6 +21236,89 @@
       <c r="V314" s="2"/>
       <c r="W314" s="2"/>
       <c r="X314" s="2"/>
+      <c r="Y314" s="2"/>
+      <c r="Z314" s="2"/>
+    </row>
+    <row r="315" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A315" s="2"/>
+      <c r="B315" s="2"/>
+      <c r="C315" s="2"/>
+      <c r="D315" s="2"/>
+      <c r="E315" s="2"/>
+      <c r="F315" s="2"/>
+      <c r="G315" s="2"/>
+      <c r="H315" s="2"/>
+      <c r="I315" s="2"/>
+      <c r="J315" s="2"/>
+      <c r="K315" s="2"/>
+      <c r="L315" s="2"/>
+      <c r="M315" s="2"/>
+      <c r="N315" s="2"/>
+      <c r="O315" s="2"/>
+      <c r="P315" s="2"/>
+      <c r="Q315" s="2"/>
+      <c r="R315" s="2"/>
+      <c r="S315" s="2"/>
+      <c r="T315" s="2"/>
+      <c r="U315" s="2"/>
+      <c r="V315" s="2"/>
+      <c r="W315" s="2"/>
+      <c r="X315" s="2"/>
+      <c r="Y315" s="2"/>
+      <c r="Z315" s="2"/>
+    </row>
+    <row r="316" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A316" s="2"/>
+      <c r="B316" s="2"/>
+      <c r="C316" s="2"/>
+      <c r="D316" s="2"/>
+      <c r="E316" s="2"/>
+      <c r="F316" s="2"/>
+      <c r="G316" s="2"/>
+      <c r="H316" s="2"/>
+      <c r="I316" s="2"/>
+      <c r="J316" s="2"/>
+      <c r="K316" s="2"/>
+      <c r="L316" s="2"/>
+      <c r="M316" s="2"/>
+      <c r="N316" s="2"/>
+      <c r="O316" s="2"/>
+      <c r="P316" s="2"/>
+      <c r="Q316" s="2"/>
+      <c r="R316" s="2"/>
+      <c r="S316" s="2"/>
+      <c r="T316" s="2"/>
+      <c r="U316" s="2"/>
+      <c r="V316" s="2"/>
+      <c r="W316" s="2"/>
+      <c r="X316" s="2"/>
+      <c r="Y316" s="2"/>
+    </row>
+    <row r="317" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A317" s="2"/>
+      <c r="B317" s="2"/>
+      <c r="C317" s="2"/>
+      <c r="D317" s="2"/>
+      <c r="E317" s="2"/>
+      <c r="F317" s="2"/>
+      <c r="G317" s="2"/>
+      <c r="H317" s="2"/>
+      <c r="I317" s="2"/>
+      <c r="J317" s="2"/>
+      <c r="K317" s="2"/>
+      <c r="L317" s="2"/>
+      <c r="M317" s="2"/>
+      <c r="N317" s="2"/>
+      <c r="O317" s="2"/>
+      <c r="P317" s="2"/>
+      <c r="Q317" s="2"/>
+      <c r="R317" s="2"/>
+      <c r="S317" s="2"/>
+      <c r="T317" s="2"/>
+      <c r="U317" s="2"/>
+      <c r="V317" s="2"/>
+      <c r="W317" s="2"/>
+      <c r="X317" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Corrections made. Corrected E_chiral. It was 31000. Also small corrections to the setUpParametric file
</commit_message>
<xml_diff>
--- a/simulationsDiary.xlsx
+++ b/simulationsDiary.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="385" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="388" uniqueCount="117">
   <si>
     <t>typeOfModel</t>
   </si>
@@ -359,6 +359,15 @@
   <si>
     <t>Even when the dofs 1,2 are the only ones contrained, there is still not free UR3 of the node</t>
   </si>
+  <si>
+    <t>To use equations is not the right approach</t>
+  </si>
+  <si>
+    <t>Come back to simply tyre as a way of modelling the connection and try to expand the model</t>
+  </si>
+  <si>
+    <t>Damp</t>
+  </si>
 </sst>
 </file>
 
@@ -418,7 +427,10 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="11">
+  <dxfs count="12">
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -484,7 +496,7 @@
     <tableColumn id="13" name="C3"/>
     <tableColumn id="14" name="eOverB"/>
     <tableColumn id="15" name="tChiral"/>
-    <tableColumn id="26" name="typeBC" dataDxfId="10"/>
+    <tableColumn id="26" name="typeBC" dataDxfId="11"/>
     <tableColumn id="16" name="typeOfLoad"/>
     <tableColumn id="17" name="zPos"/>
     <tableColumn id="18" name="Force Magnitude"/>
@@ -492,18 +504,18 @@
     <tableColumn id="20" name="fineSize"/>
     <tableColumn id="21" name="MAX U2 (cm)"/>
     <tableColumn id="22" name="MAX UR1 (rad)"/>
-    <tableColumn id="24" name="τ/T" dataDxfId="9"/>
+    <tableColumn id="24" name="τ/T" dataDxfId="10"/>
     <tableColumn id="23" name="DESCRIPTION"/>
-    <tableColumn id="25" name="Next step" dataDxfId="8"/>
+    <tableColumn id="25" name="Next step" dataDxfId="9"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table13" displayName="Table13" ref="A1:Y12" totalsRowShown="0">
-  <autoFilter ref="A1:Y12"/>
-  <tableColumns count="25">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table13" displayName="Table13" ref="A1:Z12" totalsRowShown="0">
+  <autoFilter ref="A1:Z12"/>
+  <tableColumns count="26">
     <tableColumn id="3" name="N"/>
     <tableColumn id="4" name="M"/>
     <tableColumn id="5" name="r"/>
@@ -513,7 +525,7 @@
     <tableColumn id="13" name="C3"/>
     <tableColumn id="14" name="eOverB"/>
     <tableColumn id="15" name="tChiral"/>
-    <tableColumn id="26" name="typeBC" dataDxfId="7"/>
+    <tableColumn id="26" name="typeBC" dataDxfId="8"/>
     <tableColumn id="16" name="typeOfLoad"/>
     <tableColumn id="17" name="zPos"/>
     <tableColumn id="18" name="Force Magnitude"/>
@@ -521,14 +533,15 @@
     <tableColumn id="20" name="fineSize"/>
     <tableColumn id="21" name="MAX U2 (cm)"/>
     <tableColumn id="22" name="MAX UR1 (rad)"/>
-    <tableColumn id="27" name="Connection type" dataDxfId="4"/>
-    <tableColumn id="2" name="Coupling dofs" dataDxfId="5"/>
-    <tableColumn id="28" name="Condition inner nodes" dataDxfId="3"/>
-    <tableColumn id="24" name="τ/T" dataDxfId="2"/>
+    <tableColumn id="27" name="Connection type" dataDxfId="7"/>
+    <tableColumn id="2" name="Coupling dofs" dataDxfId="6"/>
+    <tableColumn id="28" name="Condition inner nodes" dataDxfId="5"/>
+    <tableColumn id="1" name="Damp" dataDxfId="0"/>
+    <tableColumn id="24" name="τ/T" dataDxfId="4"/>
     <tableColumn id="23" name="DESCRIPTION"/>
-    <tableColumn id="25" name="Next step" dataDxfId="6"/>
-    <tableColumn id="29" name="Conclusions" dataDxfId="1"/>
-    <tableColumn id="30" name="Additional conclusion" dataDxfId="0"/>
+    <tableColumn id="25" name="Next step" dataDxfId="3"/>
+    <tableColumn id="29" name="Conclusions" dataDxfId="2"/>
+    <tableColumn id="30" name="Additional conclusion" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -21741,10 +21754,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:BJ298"/>
+  <dimension ref="A1:BK298"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="W11" sqref="W11"/>
+    <sheetView tabSelected="1" topLeftCell="L1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="W8" sqref="W8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -21757,17 +21770,18 @@
     <col min="13" max="13" width="12.5703125" customWidth="1"/>
     <col min="14" max="14" width="10.28515625" customWidth="1"/>
     <col min="15" max="15" width="14.28515625" customWidth="1"/>
-    <col min="16" max="16" width="14.42578125" customWidth="1"/>
-    <col min="17" max="17" width="13.140625" customWidth="1"/>
+    <col min="16" max="16" width="11.5703125" customWidth="1"/>
+    <col min="17" max="17" width="8" customWidth="1"/>
     <col min="19" max="19" width="13.85546875" customWidth="1"/>
-    <col min="20" max="21" width="20.85546875" customWidth="1"/>
-    <col min="22" max="22" width="49.85546875" customWidth="1"/>
-    <col min="23" max="23" width="32.85546875" customWidth="1"/>
-    <col min="24" max="24" width="29.140625" customWidth="1"/>
-    <col min="25" max="25" width="41.5703125" customWidth="1"/>
+    <col min="20" max="21" width="9.85546875" customWidth="1"/>
+    <col min="22" max="22" width="7.28515625" customWidth="1"/>
+    <col min="23" max="23" width="49.85546875" customWidth="1"/>
+    <col min="24" max="24" width="32.85546875" customWidth="1"/>
+    <col min="25" max="25" width="29.140625" customWidth="1"/>
+    <col min="26" max="26" width="41.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:62" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:63" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -21829,22 +21843,25 @@
         <v>84</v>
       </c>
       <c r="U1" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="V1" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="V1" t="s">
+      <c r="W1" t="s">
         <v>20</v>
       </c>
-      <c r="W1" t="s">
+      <c r="X1" t="s">
         <v>52</v>
       </c>
-      <c r="X1" t="s">
+      <c r="Y1" t="s">
         <v>94</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="Z1" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="2" spans="1:62" s="2" customFormat="1" ht="65.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:63" s="2" customFormat="1" ht="65.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>4</v>
       </c>
@@ -21903,16 +21920,19 @@
         <v>85</v>
       </c>
       <c r="U2" s="2">
+        <v>0</v>
+      </c>
+      <c r="V2" s="2">
         <v>1</v>
       </c>
-      <c r="V2" s="2" t="s">
+      <c r="W2" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="W2" s="2" t="s">
+      <c r="X2" s="2" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="3" spans="1:62" ht="76.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:63" ht="76.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>4</v>
       </c>
@@ -21974,16 +21994,18 @@
       <c r="U3" s="2">
         <v>0</v>
       </c>
-      <c r="V3" s="2" t="s">
+      <c r="V3" s="2">
+        <v>0</v>
+      </c>
+      <c r="W3" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="W3" s="2" t="s">
+      <c r="X3" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="X3" s="2" t="s">
+      <c r="Y3" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="Y3" s="2"/>
       <c r="Z3" s="2"/>
       <c r="AA3" s="2"/>
       <c r="AB3" s="2"/>
@@ -22021,8 +22043,9 @@
       <c r="BH3" s="2"/>
       <c r="BI3" s="2"/>
       <c r="BJ3" s="2"/>
-    </row>
-    <row r="4" spans="1:62" ht="30" x14ac:dyDescent="0.25">
+      <c r="BK3" s="2"/>
+    </row>
+    <row r="4" spans="1:63" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>4</v>
       </c>
@@ -22084,13 +22107,15 @@
       <c r="U4" s="2">
         <v>0</v>
       </c>
-      <c r="V4" s="2" t="s">
+      <c r="V4" s="2">
+        <v>0</v>
+      </c>
+      <c r="W4" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="W4" s="2" t="s">
+      <c r="X4" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="X4" s="2"/>
       <c r="Y4" s="2"/>
       <c r="Z4" s="2"/>
       <c r="AA4" s="2"/>
@@ -22129,8 +22154,9 @@
       <c r="BH4" s="2"/>
       <c r="BI4" s="2"/>
       <c r="BJ4" s="2"/>
-    </row>
-    <row r="5" spans="1:62" ht="75" x14ac:dyDescent="0.25">
+      <c r="BK4" s="2"/>
+    </row>
+    <row r="5" spans="1:63" ht="60" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -22190,21 +22216,23 @@
         <v>85</v>
       </c>
       <c r="U5" s="2">
+        <v>0</v>
+      </c>
+      <c r="V5" s="2">
         <v>1</v>
       </c>
-      <c r="V5" s="2" t="s">
+      <c r="W5" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="W5" s="2" t="s">
+      <c r="X5" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="X5" s="2" t="s">
+      <c r="Y5" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="Y5" s="2" t="s">
+      <c r="Z5" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="Z5" s="2"/>
       <c r="AA5" s="2"/>
       <c r="AB5" s="2"/>
       <c r="AC5" s="2"/>
@@ -22240,8 +22268,9 @@
       <c r="BG5" s="2"/>
       <c r="BH5" s="2"/>
       <c r="BI5" s="2"/>
-    </row>
-    <row r="6" spans="1:62" ht="45" x14ac:dyDescent="0.25">
+      <c r="BJ5" s="2"/>
+    </row>
+    <row r="6" spans="1:63" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>4</v>
       </c>
@@ -22301,18 +22330,20 @@
         <v>87</v>
       </c>
       <c r="U6" s="2">
+        <v>0</v>
+      </c>
+      <c r="V6" s="2">
         <v>1</v>
       </c>
-      <c r="V6" s="2" t="s">
+      <c r="W6" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="W6" s="2" t="s">
+      <c r="X6" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="X6" s="2" t="s">
+      <c r="Y6" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="Y6" s="2"/>
       <c r="Z6" s="2"/>
       <c r="AA6" s="2"/>
       <c r="AB6" s="2"/>
@@ -22349,8 +22380,9 @@
       <c r="BG6" s="2"/>
       <c r="BH6" s="2"/>
       <c r="BI6" s="2"/>
-    </row>
-    <row r="7" spans="1:62" ht="30" x14ac:dyDescent="0.25">
+      <c r="BJ6" s="2"/>
+    </row>
+    <row r="7" spans="1:63" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>4</v>
       </c>
@@ -22410,15 +22442,17 @@
         <v>87</v>
       </c>
       <c r="U7" s="2">
+        <v>0</v>
+      </c>
+      <c r="V7" s="2">
         <v>1</v>
       </c>
-      <c r="V7" s="2" t="s">
+      <c r="W7" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="W7" s="2" t="s">
+      <c r="X7" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="X7" s="2"/>
       <c r="Y7" s="2"/>
       <c r="Z7" s="2"/>
       <c r="AA7" s="2"/>
@@ -22456,8 +22490,9 @@
       <c r="BG7" s="2"/>
       <c r="BH7" s="2"/>
       <c r="BI7" s="2"/>
-    </row>
-    <row r="8" spans="1:62" ht="30" x14ac:dyDescent="0.25">
+      <c r="BJ7" s="2"/>
+    </row>
+    <row r="8" spans="1:63" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>4</v>
       </c>
@@ -22517,15 +22552,17 @@
         <v>87</v>
       </c>
       <c r="U8" s="2">
+        <v>0</v>
+      </c>
+      <c r="V8" s="2">
         <v>1</v>
       </c>
-      <c r="V8" s="2" t="s">
+      <c r="W8" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="W8" s="2" t="s">
+      <c r="X8" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="X8" s="2"/>
       <c r="Y8" s="2"/>
       <c r="Z8" s="2"/>
       <c r="AA8" s="2"/>
@@ -22562,8 +22599,9 @@
       <c r="BF8" s="2"/>
       <c r="BG8" s="2"/>
       <c r="BH8" s="2"/>
-    </row>
-    <row r="9" spans="1:62" ht="45" x14ac:dyDescent="0.25">
+      <c r="BI8" s="2"/>
+    </row>
+    <row r="9" spans="1:63" ht="45" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>4</v>
       </c>
@@ -22623,15 +22661,17 @@
         <v>87</v>
       </c>
       <c r="U9" s="2">
+        <v>0</v>
+      </c>
+      <c r="V9" s="2">
         <v>1</v>
       </c>
-      <c r="V9" s="2" t="s">
+      <c r="W9" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="W9" s="2" t="s">
+      <c r="X9" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="X9" s="2"/>
       <c r="Y9" s="2"/>
       <c r="Z9" s="2"/>
       <c r="AA9" s="2"/>
@@ -22668,8 +22708,9 @@
       <c r="BF9" s="2"/>
       <c r="BG9" s="2"/>
       <c r="BH9" s="2"/>
-    </row>
-    <row r="10" spans="1:62" ht="30" x14ac:dyDescent="0.25">
+      <c r="BI9" s="2"/>
+    </row>
+    <row r="10" spans="1:63" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>4</v>
       </c>
@@ -22729,12 +22770,14 @@
         <v>87</v>
       </c>
       <c r="U10" s="2">
+        <v>0</v>
+      </c>
+      <c r="V10" s="2">
         <v>1</v>
       </c>
-      <c r="V10" s="2" t="s">
+      <c r="W10" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="W10" s="2"/>
       <c r="X10" s="2"/>
       <c r="Y10" s="2"/>
       <c r="Z10" s="2"/>
@@ -22772,8 +22815,9 @@
       <c r="BF10" s="2"/>
       <c r="BG10" s="2"/>
       <c r="BH10" s="2"/>
-    </row>
-    <row r="11" spans="1:62" ht="30" x14ac:dyDescent="0.25">
+      <c r="BI10" s="2"/>
+    </row>
+    <row r="11" spans="1:63" ht="45" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>4</v>
       </c>
@@ -22833,15 +22877,21 @@
         <v>87</v>
       </c>
       <c r="U11" s="2">
+        <v>0</v>
+      </c>
+      <c r="V11" s="2">
         <v>1</v>
       </c>
-      <c r="V11" s="2" t="s">
+      <c r="W11" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="W11" s="2"/>
-      <c r="X11" s="2"/>
+      <c r="X11" s="2" t="s">
+        <v>115</v>
+      </c>
       <c r="Y11" s="2"/>
-      <c r="Z11" s="2"/>
+      <c r="Z11" s="2" t="s">
+        <v>114</v>
+      </c>
       <c r="AA11" s="2"/>
       <c r="AB11" s="2"/>
       <c r="AC11" s="2"/>
@@ -22876,10 +22926,11 @@
       <c r="BF11" s="2"/>
       <c r="BG11" s="2"/>
       <c r="BH11" s="2"/>
-    </row>
-    <row r="12" spans="1:62" ht="30" x14ac:dyDescent="0.25">
+      <c r="BI11" s="2"/>
+    </row>
+    <row r="12" spans="1:63" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B12" s="2">
         <v>3</v>
@@ -22918,7 +22969,7 @@
         <v>-2000</v>
       </c>
       <c r="N12" s="2">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="O12" s="2">
         <v>3</v>
@@ -22928,17 +22979,15 @@
       </c>
       <c r="Q12" s="2"/>
       <c r="R12" s="2" t="s">
-        <v>108</v>
+        <v>87</v>
       </c>
       <c r="S12" s="2" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="T12" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="U12" s="2">
-        <v>1</v>
-      </c>
+      <c r="U12" s="2"/>
       <c r="V12" s="2"/>
       <c r="W12" s="2"/>
       <c r="X12" s="2"/>
@@ -22977,8 +23026,9 @@
       <c r="BE12" s="2"/>
       <c r="BF12" s="2"/>
       <c r="BG12" s="2"/>
-    </row>
-    <row r="13" spans="1:62" x14ac:dyDescent="0.25">
+      <c r="BH12" s="2"/>
+    </row>
+    <row r="13" spans="1:63" x14ac:dyDescent="0.25">
       <c r="A13" s="2"/>
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
@@ -23037,8 +23087,9 @@
       <c r="BE13" s="2"/>
       <c r="BF13" s="2"/>
       <c r="BG13" s="2"/>
-    </row>
-    <row r="14" spans="1:62" x14ac:dyDescent="0.25">
+      <c r="BH13" s="2"/>
+    </row>
+    <row r="14" spans="1:63" x14ac:dyDescent="0.25">
       <c r="A14" s="2"/>
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
@@ -23097,8 +23148,9 @@
       <c r="BE14" s="2"/>
       <c r="BF14" s="2"/>
       <c r="BG14" s="2"/>
-    </row>
-    <row r="15" spans="1:62" x14ac:dyDescent="0.25">
+      <c r="BH14" s="2"/>
+    </row>
+    <row r="15" spans="1:63" x14ac:dyDescent="0.25">
       <c r="A15" s="2"/>
       <c r="B15" s="2"/>
       <c r="C15" s="2"/>
@@ -23157,8 +23209,9 @@
       <c r="BE15" s="2"/>
       <c r="BF15" s="2"/>
       <c r="BG15" s="2"/>
-    </row>
-    <row r="16" spans="1:62" x14ac:dyDescent="0.25">
+      <c r="BH15" s="2"/>
+    </row>
+    <row r="16" spans="1:63" x14ac:dyDescent="0.25">
       <c r="A16" s="2"/>
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>
@@ -23217,8 +23270,9 @@
       <c r="BE16" s="2"/>
       <c r="BF16" s="2"/>
       <c r="BG16" s="2"/>
-    </row>
-    <row r="17" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="BH16" s="2"/>
+    </row>
+    <row r="17" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A17" s="2"/>
       <c r="B17" s="2"/>
       <c r="C17" s="2"/>
@@ -23277,8 +23331,9 @@
       <c r="BE17" s="2"/>
       <c r="BF17" s="2"/>
       <c r="BG17" s="2"/>
-    </row>
-    <row r="18" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="BH17" s="2"/>
+    </row>
+    <row r="18" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A18" s="2"/>
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
@@ -23337,8 +23392,9 @@
       <c r="BE18" s="2"/>
       <c r="BF18" s="2"/>
       <c r="BG18" s="2"/>
-    </row>
-    <row r="19" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="BH18" s="2"/>
+    </row>
+    <row r="19" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A19" s="2"/>
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
@@ -23397,8 +23453,9 @@
       <c r="BE19" s="2"/>
       <c r="BF19" s="2"/>
       <c r="BG19" s="2"/>
-    </row>
-    <row r="20" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="BH19" s="2"/>
+    </row>
+    <row r="20" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A20" s="2"/>
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
@@ -23457,8 +23514,9 @@
       <c r="BE20" s="2"/>
       <c r="BF20" s="2"/>
       <c r="BG20" s="2"/>
-    </row>
-    <row r="21" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="BH20" s="2"/>
+    </row>
+    <row r="21" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A21" s="2"/>
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
@@ -23517,8 +23575,9 @@
       <c r="BE21" s="2"/>
       <c r="BF21" s="2"/>
       <c r="BG21" s="2"/>
-    </row>
-    <row r="22" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="BH21" s="2"/>
+    </row>
+    <row r="22" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A22" s="2"/>
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
@@ -23577,8 +23636,9 @@
       <c r="BE22" s="2"/>
       <c r="BF22" s="2"/>
       <c r="BG22" s="2"/>
-    </row>
-    <row r="23" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="BH22" s="2"/>
+    </row>
+    <row r="23" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A23" s="2"/>
       <c r="B23" s="2"/>
       <c r="C23" s="2"/>
@@ -23637,8 +23697,9 @@
       <c r="BE23" s="2"/>
       <c r="BF23" s="2"/>
       <c r="BG23" s="2"/>
-    </row>
-    <row r="24" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="BH23" s="2"/>
+    </row>
+    <row r="24" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A24" s="2"/>
       <c r="B24" s="2"/>
       <c r="C24" s="2"/>
@@ -23697,8 +23758,9 @@
       <c r="BE24" s="2"/>
       <c r="BF24" s="2"/>
       <c r="BG24" s="2"/>
-    </row>
-    <row r="25" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="BH24" s="2"/>
+    </row>
+    <row r="25" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A25" s="2"/>
       <c r="B25" s="2"/>
       <c r="C25" s="2"/>
@@ -23757,8 +23819,9 @@
       <c r="BE25" s="2"/>
       <c r="BF25" s="2"/>
       <c r="BG25" s="2"/>
-    </row>
-    <row r="26" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="BH25" s="2"/>
+    </row>
+    <row r="26" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A26" s="2"/>
       <c r="B26" s="2"/>
       <c r="C26" s="2"/>
@@ -23817,8 +23880,9 @@
       <c r="BE26" s="2"/>
       <c r="BF26" s="2"/>
       <c r="BG26" s="2"/>
-    </row>
-    <row r="27" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="BH26" s="2"/>
+    </row>
+    <row r="27" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A27" s="2"/>
       <c r="B27" s="2"/>
       <c r="C27" s="2"/>
@@ -23877,8 +23941,9 @@
       <c r="BE27" s="2"/>
       <c r="BF27" s="2"/>
       <c r="BG27" s="2"/>
-    </row>
-    <row r="28" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="BH27" s="2"/>
+    </row>
+    <row r="28" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A28" s="2"/>
       <c r="B28" s="2"/>
       <c r="C28" s="2"/>
@@ -23937,8 +24002,9 @@
       <c r="BE28" s="2"/>
       <c r="BF28" s="2"/>
       <c r="BG28" s="2"/>
-    </row>
-    <row r="29" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="BH28" s="2"/>
+    </row>
+    <row r="29" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A29" s="2"/>
       <c r="B29" s="2"/>
       <c r="C29" s="2"/>
@@ -23997,8 +24063,9 @@
       <c r="BE29" s="2"/>
       <c r="BF29" s="2"/>
       <c r="BG29" s="2"/>
-    </row>
-    <row r="30" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="BH29" s="2"/>
+    </row>
+    <row r="30" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A30" s="2"/>
       <c r="B30" s="2"/>
       <c r="C30" s="2"/>
@@ -24057,8 +24124,9 @@
       <c r="BE30" s="2"/>
       <c r="BF30" s="2"/>
       <c r="BG30" s="2"/>
-    </row>
-    <row r="31" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="BH30" s="2"/>
+    </row>
+    <row r="31" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A31" s="2"/>
       <c r="B31" s="2"/>
       <c r="C31" s="2"/>
@@ -24117,8 +24185,9 @@
       <c r="BE31" s="2"/>
       <c r="BF31" s="2"/>
       <c r="BG31" s="2"/>
-    </row>
-    <row r="32" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="BH31" s="2"/>
+    </row>
+    <row r="32" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A32" s="2"/>
       <c r="B32" s="2"/>
       <c r="C32" s="2"/>
@@ -24177,8 +24246,9 @@
       <c r="BE32" s="2"/>
       <c r="BF32" s="2"/>
       <c r="BG32" s="2"/>
-    </row>
-    <row r="33" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="BH32" s="2"/>
+    </row>
+    <row r="33" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A33" s="2"/>
       <c r="B33" s="2"/>
       <c r="C33" s="2"/>
@@ -24237,8 +24307,9 @@
       <c r="BE33" s="2"/>
       <c r="BF33" s="2"/>
       <c r="BG33" s="2"/>
-    </row>
-    <row r="34" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="BH33" s="2"/>
+    </row>
+    <row r="34" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A34" s="2"/>
       <c r="B34" s="2"/>
       <c r="C34" s="2"/>
@@ -24297,8 +24368,9 @@
       <c r="BE34" s="2"/>
       <c r="BF34" s="2"/>
       <c r="BG34" s="2"/>
-    </row>
-    <row r="35" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="BH34" s="2"/>
+    </row>
+    <row r="35" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A35" s="2"/>
       <c r="B35" s="2"/>
       <c r="C35" s="2"/>
@@ -24357,8 +24429,9 @@
       <c r="BE35" s="2"/>
       <c r="BF35" s="2"/>
       <c r="BG35" s="2"/>
-    </row>
-    <row r="36" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="BH35" s="2"/>
+    </row>
+    <row r="36" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A36" s="2"/>
       <c r="B36" s="2"/>
       <c r="C36" s="2"/>
@@ -24417,8 +24490,9 @@
       <c r="BE36" s="2"/>
       <c r="BF36" s="2"/>
       <c r="BG36" s="2"/>
-    </row>
-    <row r="37" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="BH36" s="2"/>
+    </row>
+    <row r="37" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A37" s="2"/>
       <c r="B37" s="2"/>
       <c r="C37" s="2"/>
@@ -24477,8 +24551,9 @@
       <c r="BE37" s="2"/>
       <c r="BF37" s="2"/>
       <c r="BG37" s="2"/>
-    </row>
-    <row r="38" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="BH37" s="2"/>
+    </row>
+    <row r="38" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A38" s="2"/>
       <c r="B38" s="2"/>
       <c r="C38" s="2"/>
@@ -24537,8 +24612,9 @@
       <c r="BE38" s="2"/>
       <c r="BF38" s="2"/>
       <c r="BG38" s="2"/>
-    </row>
-    <row r="39" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="BH38" s="2"/>
+    </row>
+    <row r="39" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A39" s="2"/>
       <c r="B39" s="2"/>
       <c r="C39" s="2"/>
@@ -24597,8 +24673,9 @@
       <c r="BE39" s="2"/>
       <c r="BF39" s="2"/>
       <c r="BG39" s="2"/>
-    </row>
-    <row r="40" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="BH39" s="2"/>
+    </row>
+    <row r="40" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A40" s="2"/>
       <c r="B40" s="2"/>
       <c r="C40" s="2"/>
@@ -24657,8 +24734,9 @@
       <c r="BE40" s="2"/>
       <c r="BF40" s="2"/>
       <c r="BG40" s="2"/>
-    </row>
-    <row r="41" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="BH40" s="2"/>
+    </row>
+    <row r="41" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A41" s="2"/>
       <c r="B41" s="2"/>
       <c r="C41" s="2"/>
@@ -24717,8 +24795,9 @@
       <c r="BE41" s="2"/>
       <c r="BF41" s="2"/>
       <c r="BG41" s="2"/>
-    </row>
-    <row r="42" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="BH41" s="2"/>
+    </row>
+    <row r="42" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A42" s="2"/>
       <c r="B42" s="2"/>
       <c r="C42" s="2"/>
@@ -24777,8 +24856,9 @@
       <c r="BE42" s="2"/>
       <c r="BF42" s="2"/>
       <c r="BG42" s="2"/>
-    </row>
-    <row r="43" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="BH42" s="2"/>
+    </row>
+    <row r="43" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A43" s="2"/>
       <c r="B43" s="2"/>
       <c r="C43" s="2"/>
@@ -24837,8 +24917,9 @@
       <c r="BE43" s="2"/>
       <c r="BF43" s="2"/>
       <c r="BG43" s="2"/>
-    </row>
-    <row r="44" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="BH43" s="2"/>
+    </row>
+    <row r="44" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A44" s="2"/>
       <c r="B44" s="2"/>
       <c r="C44" s="2"/>
@@ -24897,8 +24978,9 @@
       <c r="BE44" s="2"/>
       <c r="BF44" s="2"/>
       <c r="BG44" s="2"/>
-    </row>
-    <row r="45" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="BH44" s="2"/>
+    </row>
+    <row r="45" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A45" s="2"/>
       <c r="B45" s="2"/>
       <c r="C45" s="2"/>
@@ -24957,8 +25039,9 @@
       <c r="BE45" s="2"/>
       <c r="BF45" s="2"/>
       <c r="BG45" s="2"/>
-    </row>
-    <row r="46" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="BH45" s="2"/>
+    </row>
+    <row r="46" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A46" s="2"/>
       <c r="B46" s="2"/>
       <c r="C46" s="2"/>
@@ -25017,8 +25100,9 @@
       <c r="BE46" s="2"/>
       <c r="BF46" s="2"/>
       <c r="BG46" s="2"/>
-    </row>
-    <row r="47" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="BH46" s="2"/>
+    </row>
+    <row r="47" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A47" s="2"/>
       <c r="B47" s="2"/>
       <c r="C47" s="2"/>
@@ -25077,8 +25161,9 @@
       <c r="BE47" s="2"/>
       <c r="BF47" s="2"/>
       <c r="BG47" s="2"/>
-    </row>
-    <row r="48" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="BH47" s="2"/>
+    </row>
+    <row r="48" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A48" s="2"/>
       <c r="B48" s="2"/>
       <c r="C48" s="2"/>
@@ -25137,8 +25222,9 @@
       <c r="BE48" s="2"/>
       <c r="BF48" s="2"/>
       <c r="BG48" s="2"/>
-    </row>
-    <row r="49" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="BH48" s="2"/>
+    </row>
+    <row r="49" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A49" s="2"/>
       <c r="B49" s="2"/>
       <c r="C49" s="2"/>
@@ -25197,8 +25283,9 @@
       <c r="BE49" s="2"/>
       <c r="BF49" s="2"/>
       <c r="BG49" s="2"/>
-    </row>
-    <row r="50" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="BH49" s="2"/>
+    </row>
+    <row r="50" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A50" s="2"/>
       <c r="B50" s="2"/>
       <c r="C50" s="2"/>
@@ -25257,8 +25344,9 @@
       <c r="BE50" s="2"/>
       <c r="BF50" s="2"/>
       <c r="BG50" s="2"/>
-    </row>
-    <row r="51" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="BH50" s="2"/>
+    </row>
+    <row r="51" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A51" s="2"/>
       <c r="B51" s="2"/>
       <c r="C51" s="2"/>
@@ -25317,8 +25405,9 @@
       <c r="BE51" s="2"/>
       <c r="BF51" s="2"/>
       <c r="BG51" s="2"/>
-    </row>
-    <row r="52" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="BH51" s="2"/>
+    </row>
+    <row r="52" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A52" s="2"/>
       <c r="B52" s="2"/>
       <c r="C52" s="2"/>
@@ -25377,8 +25466,9 @@
       <c r="BE52" s="2"/>
       <c r="BF52" s="2"/>
       <c r="BG52" s="2"/>
-    </row>
-    <row r="53" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="BH52" s="2"/>
+    </row>
+    <row r="53" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A53" s="2"/>
       <c r="B53" s="2"/>
       <c r="C53" s="2"/>
@@ -25437,8 +25527,9 @@
       <c r="BE53" s="2"/>
       <c r="BF53" s="2"/>
       <c r="BG53" s="2"/>
-    </row>
-    <row r="54" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="BH53" s="2"/>
+    </row>
+    <row r="54" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A54" s="2"/>
       <c r="B54" s="2"/>
       <c r="C54" s="2"/>
@@ -25497,8 +25588,9 @@
       <c r="BE54" s="2"/>
       <c r="BF54" s="2"/>
       <c r="BG54" s="2"/>
-    </row>
-    <row r="55" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="BH54" s="2"/>
+    </row>
+    <row r="55" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A55" s="2"/>
       <c r="B55" s="2"/>
       <c r="C55" s="2"/>
@@ -25557,8 +25649,9 @@
       <c r="BE55" s="2"/>
       <c r="BF55" s="2"/>
       <c r="BG55" s="2"/>
-    </row>
-    <row r="56" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="BH55" s="2"/>
+    </row>
+    <row r="56" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A56" s="2"/>
       <c r="B56" s="2"/>
       <c r="C56" s="2"/>
@@ -25617,8 +25710,9 @@
       <c r="BE56" s="2"/>
       <c r="BF56" s="2"/>
       <c r="BG56" s="2"/>
-    </row>
-    <row r="57" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="BH56" s="2"/>
+    </row>
+    <row r="57" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A57" s="2"/>
       <c r="B57" s="2"/>
       <c r="C57" s="2"/>
@@ -25677,8 +25771,9 @@
       <c r="BE57" s="2"/>
       <c r="BF57" s="2"/>
       <c r="BG57" s="2"/>
-    </row>
-    <row r="58" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="BH57" s="2"/>
+    </row>
+    <row r="58" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A58" s="2"/>
       <c r="B58" s="2"/>
       <c r="C58" s="2"/>
@@ -25737,8 +25832,9 @@
       <c r="BE58" s="2"/>
       <c r="BF58" s="2"/>
       <c r="BG58" s="2"/>
-    </row>
-    <row r="59" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="BH58" s="2"/>
+    </row>
+    <row r="59" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A59" s="2"/>
       <c r="B59" s="2"/>
       <c r="C59" s="2"/>
@@ -25797,8 +25893,9 @@
       <c r="BE59" s="2"/>
       <c r="BF59" s="2"/>
       <c r="BG59" s="2"/>
-    </row>
-    <row r="60" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="BH59" s="2"/>
+    </row>
+    <row r="60" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A60" s="2"/>
       <c r="B60" s="2"/>
       <c r="C60" s="2"/>
@@ -25857,8 +25954,9 @@
       <c r="BE60" s="2"/>
       <c r="BF60" s="2"/>
       <c r="BG60" s="2"/>
-    </row>
-    <row r="61" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="BH60" s="2"/>
+    </row>
+    <row r="61" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A61" s="2"/>
       <c r="B61" s="2"/>
       <c r="C61" s="2"/>
@@ -25917,8 +26015,9 @@
       <c r="BE61" s="2"/>
       <c r="BF61" s="2"/>
       <c r="BG61" s="2"/>
-    </row>
-    <row r="62" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="BH61" s="2"/>
+    </row>
+    <row r="62" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A62" s="2"/>
       <c r="B62" s="2"/>
       <c r="C62" s="2"/>
@@ -25977,8 +26076,9 @@
       <c r="BE62" s="2"/>
       <c r="BF62" s="2"/>
       <c r="BG62" s="2"/>
-    </row>
-    <row r="63" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="BH62" s="2"/>
+    </row>
+    <row r="63" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A63" s="2"/>
       <c r="B63" s="2"/>
       <c r="C63" s="2"/>
@@ -26037,8 +26137,9 @@
       <c r="BE63" s="2"/>
       <c r="BF63" s="2"/>
       <c r="BG63" s="2"/>
-    </row>
-    <row r="64" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="BH63" s="2"/>
+    </row>
+    <row r="64" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A64" s="2"/>
       <c r="B64" s="2"/>
       <c r="C64" s="2"/>
@@ -26097,8 +26198,9 @@
       <c r="BE64" s="2"/>
       <c r="BF64" s="2"/>
       <c r="BG64" s="2"/>
-    </row>
-    <row r="65" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="BH64" s="2"/>
+    </row>
+    <row r="65" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A65" s="2"/>
       <c r="B65" s="2"/>
       <c r="C65" s="2"/>
@@ -26157,8 +26259,9 @@
       <c r="BE65" s="2"/>
       <c r="BF65" s="2"/>
       <c r="BG65" s="2"/>
-    </row>
-    <row r="66" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="BH65" s="2"/>
+    </row>
+    <row r="66" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A66" s="2"/>
       <c r="B66" s="2"/>
       <c r="C66" s="2"/>
@@ -26217,8 +26320,9 @@
       <c r="BE66" s="2"/>
       <c r="BF66" s="2"/>
       <c r="BG66" s="2"/>
-    </row>
-    <row r="67" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="BH66" s="2"/>
+    </row>
+    <row r="67" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A67" s="2"/>
       <c r="B67" s="2"/>
       <c r="C67" s="2"/>
@@ -26277,8 +26381,9 @@
       <c r="BE67" s="2"/>
       <c r="BF67" s="2"/>
       <c r="BG67" s="2"/>
-    </row>
-    <row r="68" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="BH67" s="2"/>
+    </row>
+    <row r="68" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A68" s="2"/>
       <c r="B68" s="2"/>
       <c r="C68" s="2"/>
@@ -26337,8 +26442,9 @@
       <c r="BE68" s="2"/>
       <c r="BF68" s="2"/>
       <c r="BG68" s="2"/>
-    </row>
-    <row r="69" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="BH68" s="2"/>
+    </row>
+    <row r="69" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A69" s="2"/>
       <c r="B69" s="2"/>
       <c r="C69" s="2"/>
@@ -26397,8 +26503,9 @@
       <c r="BE69" s="2"/>
       <c r="BF69" s="2"/>
       <c r="BG69" s="2"/>
-    </row>
-    <row r="70" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="BH69" s="2"/>
+    </row>
+    <row r="70" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A70" s="2"/>
       <c r="B70" s="2"/>
       <c r="C70" s="2"/>
@@ -26457,8 +26564,9 @@
       <c r="BE70" s="2"/>
       <c r="BF70" s="2"/>
       <c r="BG70" s="2"/>
-    </row>
-    <row r="71" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="BH70" s="2"/>
+    </row>
+    <row r="71" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A71" s="2"/>
       <c r="B71" s="2"/>
       <c r="C71" s="2"/>
@@ -26517,8 +26625,9 @@
       <c r="BE71" s="2"/>
       <c r="BF71" s="2"/>
       <c r="BG71" s="2"/>
-    </row>
-    <row r="72" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="BH71" s="2"/>
+    </row>
+    <row r="72" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A72" s="2"/>
       <c r="B72" s="2"/>
       <c r="C72" s="2"/>
@@ -26577,8 +26686,9 @@
       <c r="BE72" s="2"/>
       <c r="BF72" s="2"/>
       <c r="BG72" s="2"/>
-    </row>
-    <row r="73" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="BH72" s="2"/>
+    </row>
+    <row r="73" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A73" s="2"/>
       <c r="B73" s="2"/>
       <c r="C73" s="2"/>
@@ -26637,8 +26747,9 @@
       <c r="BE73" s="2"/>
       <c r="BF73" s="2"/>
       <c r="BG73" s="2"/>
-    </row>
-    <row r="74" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="BH73" s="2"/>
+    </row>
+    <row r="74" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A74" s="2"/>
       <c r="B74" s="2"/>
       <c r="C74" s="2"/>
@@ -26697,8 +26808,9 @@
       <c r="BE74" s="2"/>
       <c r="BF74" s="2"/>
       <c r="BG74" s="2"/>
-    </row>
-    <row r="75" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="BH74" s="2"/>
+    </row>
+    <row r="75" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A75" s="2"/>
       <c r="B75" s="2"/>
       <c r="C75" s="2"/>
@@ -26757,8 +26869,9 @@
       <c r="BE75" s="2"/>
       <c r="BF75" s="2"/>
       <c r="BG75" s="2"/>
-    </row>
-    <row r="76" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="BH75" s="2"/>
+    </row>
+    <row r="76" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A76" s="2"/>
       <c r="B76" s="2"/>
       <c r="C76" s="2"/>
@@ -26817,8 +26930,9 @@
       <c r="BE76" s="2"/>
       <c r="BF76" s="2"/>
       <c r="BG76" s="2"/>
-    </row>
-    <row r="77" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="BH76" s="2"/>
+    </row>
+    <row r="77" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A77" s="2"/>
       <c r="B77" s="2"/>
       <c r="C77" s="2"/>
@@ -26877,8 +26991,9 @@
       <c r="BE77" s="2"/>
       <c r="BF77" s="2"/>
       <c r="BG77" s="2"/>
-    </row>
-    <row r="78" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="BH77" s="2"/>
+    </row>
+    <row r="78" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A78" s="2"/>
       <c r="B78" s="2"/>
       <c r="C78" s="2"/>
@@ -26937,8 +27052,9 @@
       <c r="BE78" s="2"/>
       <c r="BF78" s="2"/>
       <c r="BG78" s="2"/>
-    </row>
-    <row r="79" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="BH78" s="2"/>
+    </row>
+    <row r="79" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A79" s="2"/>
       <c r="B79" s="2"/>
       <c r="C79" s="2"/>
@@ -26997,8 +27113,9 @@
       <c r="BE79" s="2"/>
       <c r="BF79" s="2"/>
       <c r="BG79" s="2"/>
-    </row>
-    <row r="80" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="BH79" s="2"/>
+    </row>
+    <row r="80" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A80" s="2"/>
       <c r="B80" s="2"/>
       <c r="C80" s="2"/>
@@ -27057,8 +27174,9 @@
       <c r="BE80" s="2"/>
       <c r="BF80" s="2"/>
       <c r="BG80" s="2"/>
-    </row>
-    <row r="81" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="BH80" s="2"/>
+    </row>
+    <row r="81" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A81" s="2"/>
       <c r="B81" s="2"/>
       <c r="C81" s="2"/>
@@ -27117,8 +27235,9 @@
       <c r="BE81" s="2"/>
       <c r="BF81" s="2"/>
       <c r="BG81" s="2"/>
-    </row>
-    <row r="82" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="BH81" s="2"/>
+    </row>
+    <row r="82" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A82" s="2"/>
       <c r="B82" s="2"/>
       <c r="C82" s="2"/>
@@ -27177,8 +27296,9 @@
       <c r="BE82" s="2"/>
       <c r="BF82" s="2"/>
       <c r="BG82" s="2"/>
-    </row>
-    <row r="83" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="BH82" s="2"/>
+    </row>
+    <row r="83" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A83" s="2"/>
       <c r="B83" s="2"/>
       <c r="C83" s="2"/>
@@ -27237,8 +27357,9 @@
       <c r="BE83" s="2"/>
       <c r="BF83" s="2"/>
       <c r="BG83" s="2"/>
-    </row>
-    <row r="84" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="BH83" s="2"/>
+    </row>
+    <row r="84" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A84" s="2"/>
       <c r="B84" s="2"/>
       <c r="C84" s="2"/>
@@ -27297,8 +27418,9 @@
       <c r="BE84" s="2"/>
       <c r="BF84" s="2"/>
       <c r="BG84" s="2"/>
-    </row>
-    <row r="85" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="BH84" s="2"/>
+    </row>
+    <row r="85" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A85" s="2"/>
       <c r="B85" s="2"/>
       <c r="C85" s="2"/>
@@ -27357,8 +27479,9 @@
       <c r="BE85" s="2"/>
       <c r="BF85" s="2"/>
       <c r="BG85" s="2"/>
-    </row>
-    <row r="86" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="BH85" s="2"/>
+    </row>
+    <row r="86" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A86" s="2"/>
       <c r="B86" s="2"/>
       <c r="C86" s="2"/>
@@ -27417,8 +27540,9 @@
       <c r="BE86" s="2"/>
       <c r="BF86" s="2"/>
       <c r="BG86" s="2"/>
-    </row>
-    <row r="87" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="BH86" s="2"/>
+    </row>
+    <row r="87" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A87" s="2"/>
       <c r="B87" s="2"/>
       <c r="C87" s="2"/>
@@ -27477,8 +27601,9 @@
       <c r="BE87" s="2"/>
       <c r="BF87" s="2"/>
       <c r="BG87" s="2"/>
-    </row>
-    <row r="88" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="BH87" s="2"/>
+    </row>
+    <row r="88" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A88" s="2"/>
       <c r="B88" s="2"/>
       <c r="C88" s="2"/>
@@ -27537,8 +27662,9 @@
       <c r="BE88" s="2"/>
       <c r="BF88" s="2"/>
       <c r="BG88" s="2"/>
-    </row>
-    <row r="89" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="BH88" s="2"/>
+    </row>
+    <row r="89" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A89" s="2"/>
       <c r="B89" s="2"/>
       <c r="C89" s="2"/>
@@ -27597,8 +27723,9 @@
       <c r="BE89" s="2"/>
       <c r="BF89" s="2"/>
       <c r="BG89" s="2"/>
-    </row>
-    <row r="90" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="BH89" s="2"/>
+    </row>
+    <row r="90" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A90" s="2"/>
       <c r="B90" s="2"/>
       <c r="C90" s="2"/>
@@ -27657,8 +27784,9 @@
       <c r="BE90" s="2"/>
       <c r="BF90" s="2"/>
       <c r="BG90" s="2"/>
-    </row>
-    <row r="91" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="BH90" s="2"/>
+    </row>
+    <row r="91" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A91" s="2"/>
       <c r="B91" s="2"/>
       <c r="C91" s="2"/>
@@ -27717,8 +27845,9 @@
       <c r="BE91" s="2"/>
       <c r="BF91" s="2"/>
       <c r="BG91" s="2"/>
-    </row>
-    <row r="92" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="BH91" s="2"/>
+    </row>
+    <row r="92" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A92" s="2"/>
       <c r="B92" s="2"/>
       <c r="C92" s="2"/>
@@ -27777,8 +27906,9 @@
       <c r="BE92" s="2"/>
       <c r="BF92" s="2"/>
       <c r="BG92" s="2"/>
-    </row>
-    <row r="93" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="BH92" s="2"/>
+    </row>
+    <row r="93" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A93" s="2"/>
       <c r="B93" s="2"/>
       <c r="C93" s="2"/>
@@ -27837,8 +27967,9 @@
       <c r="BE93" s="2"/>
       <c r="BF93" s="2"/>
       <c r="BG93" s="2"/>
-    </row>
-    <row r="94" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="BH93" s="2"/>
+    </row>
+    <row r="94" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A94" s="2"/>
       <c r="B94" s="2"/>
       <c r="C94" s="2"/>
@@ -27897,8 +28028,9 @@
       <c r="BE94" s="2"/>
       <c r="BF94" s="2"/>
       <c r="BG94" s="2"/>
-    </row>
-    <row r="95" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="BH94" s="2"/>
+    </row>
+    <row r="95" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A95" s="2"/>
       <c r="B95" s="2"/>
       <c r="C95" s="2"/>
@@ -27957,8 +28089,9 @@
       <c r="BE95" s="2"/>
       <c r="BF95" s="2"/>
       <c r="BG95" s="2"/>
-    </row>
-    <row r="96" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="BH95" s="2"/>
+    </row>
+    <row r="96" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A96" s="2"/>
       <c r="B96" s="2"/>
       <c r="C96" s="2"/>
@@ -28017,8 +28150,9 @@
       <c r="BE96" s="2"/>
       <c r="BF96" s="2"/>
       <c r="BG96" s="2"/>
-    </row>
-    <row r="97" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="BH96" s="2"/>
+    </row>
+    <row r="97" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A97" s="2"/>
       <c r="B97" s="2"/>
       <c r="C97" s="2"/>
@@ -28077,8 +28211,9 @@
       <c r="BE97" s="2"/>
       <c r="BF97" s="2"/>
       <c r="BG97" s="2"/>
-    </row>
-    <row r="98" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="BH97" s="2"/>
+    </row>
+    <row r="98" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A98" s="2"/>
       <c r="B98" s="2"/>
       <c r="C98" s="2"/>
@@ -28137,8 +28272,9 @@
       <c r="BE98" s="2"/>
       <c r="BF98" s="2"/>
       <c r="BG98" s="2"/>
-    </row>
-    <row r="99" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="BH98" s="2"/>
+    </row>
+    <row r="99" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A99" s="2"/>
       <c r="B99" s="2"/>
       <c r="C99" s="2"/>
@@ -28197,8 +28333,9 @@
       <c r="BE99" s="2"/>
       <c r="BF99" s="2"/>
       <c r="BG99" s="2"/>
-    </row>
-    <row r="100" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="BH99" s="2"/>
+    </row>
+    <row r="100" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A100" s="2"/>
       <c r="B100" s="2"/>
       <c r="C100" s="2"/>
@@ -28257,8 +28394,9 @@
       <c r="BE100" s="2"/>
       <c r="BF100" s="2"/>
       <c r="BG100" s="2"/>
-    </row>
-    <row r="101" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="BH100" s="2"/>
+    </row>
+    <row r="101" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A101" s="2"/>
       <c r="B101" s="2"/>
       <c r="C101" s="2"/>
@@ -28317,8 +28455,9 @@
       <c r="BE101" s="2"/>
       <c r="BF101" s="2"/>
       <c r="BG101" s="2"/>
-    </row>
-    <row r="102" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="BH101" s="2"/>
+    </row>
+    <row r="102" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A102" s="2"/>
       <c r="B102" s="2"/>
       <c r="C102" s="2"/>
@@ -28377,8 +28516,9 @@
       <c r="BE102" s="2"/>
       <c r="BF102" s="2"/>
       <c r="BG102" s="2"/>
-    </row>
-    <row r="103" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="BH102" s="2"/>
+    </row>
+    <row r="103" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A103" s="2"/>
       <c r="B103" s="2"/>
       <c r="C103" s="2"/>
@@ -28437,8 +28577,9 @@
       <c r="BE103" s="2"/>
       <c r="BF103" s="2"/>
       <c r="BG103" s="2"/>
-    </row>
-    <row r="104" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="BH103" s="2"/>
+    </row>
+    <row r="104" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A104" s="2"/>
       <c r="B104" s="2"/>
       <c r="C104" s="2"/>
@@ -28497,8 +28638,9 @@
       <c r="BE104" s="2"/>
       <c r="BF104" s="2"/>
       <c r="BG104" s="2"/>
-    </row>
-    <row r="105" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="BH104" s="2"/>
+    </row>
+    <row r="105" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A105" s="2"/>
       <c r="B105" s="2"/>
       <c r="C105" s="2"/>
@@ -28557,8 +28699,9 @@
       <c r="BE105" s="2"/>
       <c r="BF105" s="2"/>
       <c r="BG105" s="2"/>
-    </row>
-    <row r="106" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="BH105" s="2"/>
+    </row>
+    <row r="106" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A106" s="2"/>
       <c r="B106" s="2"/>
       <c r="C106" s="2"/>
@@ -28617,8 +28760,9 @@
       <c r="BE106" s="2"/>
       <c r="BF106" s="2"/>
       <c r="BG106" s="2"/>
-    </row>
-    <row r="107" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="BH106" s="2"/>
+    </row>
+    <row r="107" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A107" s="2"/>
       <c r="B107" s="2"/>
       <c r="C107" s="2"/>
@@ -28677,8 +28821,9 @@
       <c r="BE107" s="2"/>
       <c r="BF107" s="2"/>
       <c r="BG107" s="2"/>
-    </row>
-    <row r="108" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="BH107" s="2"/>
+    </row>
+    <row r="108" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A108" s="2"/>
       <c r="B108" s="2"/>
       <c r="C108" s="2"/>
@@ -28737,8 +28882,9 @@
       <c r="BE108" s="2"/>
       <c r="BF108" s="2"/>
       <c r="BG108" s="2"/>
-    </row>
-    <row r="109" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="BH108" s="2"/>
+    </row>
+    <row r="109" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A109" s="2"/>
       <c r="B109" s="2"/>
       <c r="C109" s="2"/>
@@ -28797,8 +28943,9 @@
       <c r="BE109" s="2"/>
       <c r="BF109" s="2"/>
       <c r="BG109" s="2"/>
-    </row>
-    <row r="110" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="BH109" s="2"/>
+    </row>
+    <row r="110" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A110" s="2"/>
       <c r="B110" s="2"/>
       <c r="C110" s="2"/>
@@ -28857,8 +29004,9 @@
       <c r="BE110" s="2"/>
       <c r="BF110" s="2"/>
       <c r="BG110" s="2"/>
-    </row>
-    <row r="111" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="BH110" s="2"/>
+    </row>
+    <row r="111" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A111" s="2"/>
       <c r="B111" s="2"/>
       <c r="C111" s="2"/>
@@ -28917,8 +29065,9 @@
       <c r="BE111" s="2"/>
       <c r="BF111" s="2"/>
       <c r="BG111" s="2"/>
-    </row>
-    <row r="112" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="BH111" s="2"/>
+    </row>
+    <row r="112" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A112" s="2"/>
       <c r="B112" s="2"/>
       <c r="C112" s="2"/>
@@ -28977,8 +29126,9 @@
       <c r="BE112" s="2"/>
       <c r="BF112" s="2"/>
       <c r="BG112" s="2"/>
-    </row>
-    <row r="113" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="BH112" s="2"/>
+    </row>
+    <row r="113" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A113" s="2"/>
       <c r="B113" s="2"/>
       <c r="C113" s="2"/>
@@ -29037,8 +29187,9 @@
       <c r="BE113" s="2"/>
       <c r="BF113" s="2"/>
       <c r="BG113" s="2"/>
-    </row>
-    <row r="114" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="BH113" s="2"/>
+    </row>
+    <row r="114" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A114" s="2"/>
       <c r="B114" s="2"/>
       <c r="C114" s="2"/>
@@ -29097,8 +29248,9 @@
       <c r="BE114" s="2"/>
       <c r="BF114" s="2"/>
       <c r="BG114" s="2"/>
-    </row>
-    <row r="115" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="BH114" s="2"/>
+    </row>
+    <row r="115" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A115" s="2"/>
       <c r="B115" s="2"/>
       <c r="C115" s="2"/>
@@ -29157,8 +29309,9 @@
       <c r="BE115" s="2"/>
       <c r="BF115" s="2"/>
       <c r="BG115" s="2"/>
-    </row>
-    <row r="116" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="BH115" s="2"/>
+    </row>
+    <row r="116" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A116" s="2"/>
       <c r="B116" s="2"/>
       <c r="C116" s="2"/>
@@ -29217,8 +29370,9 @@
       <c r="BE116" s="2"/>
       <c r="BF116" s="2"/>
       <c r="BG116" s="2"/>
-    </row>
-    <row r="117" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="BH116" s="2"/>
+    </row>
+    <row r="117" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A117" s="2"/>
       <c r="B117" s="2"/>
       <c r="C117" s="2"/>
@@ -29277,8 +29431,9 @@
       <c r="BE117" s="2"/>
       <c r="BF117" s="2"/>
       <c r="BG117" s="2"/>
-    </row>
-    <row r="118" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="BH117" s="2"/>
+    </row>
+    <row r="118" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A118" s="2"/>
       <c r="B118" s="2"/>
       <c r="C118" s="2"/>
@@ -29337,8 +29492,9 @@
       <c r="BE118" s="2"/>
       <c r="BF118" s="2"/>
       <c r="BG118" s="2"/>
-    </row>
-    <row r="119" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="BH118" s="2"/>
+    </row>
+    <row r="119" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A119" s="2"/>
       <c r="B119" s="2"/>
       <c r="C119" s="2"/>
@@ -29397,8 +29553,9 @@
       <c r="BE119" s="2"/>
       <c r="BF119" s="2"/>
       <c r="BG119" s="2"/>
-    </row>
-    <row r="120" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="BH119" s="2"/>
+    </row>
+    <row r="120" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A120" s="2"/>
       <c r="B120" s="2"/>
       <c r="C120" s="2"/>
@@ -29457,8 +29614,9 @@
       <c r="BE120" s="2"/>
       <c r="BF120" s="2"/>
       <c r="BG120" s="2"/>
-    </row>
-    <row r="121" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="BH120" s="2"/>
+    </row>
+    <row r="121" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A121" s="2"/>
       <c r="B121" s="2"/>
       <c r="C121" s="2"/>
@@ -29517,8 +29675,9 @@
       <c r="BE121" s="2"/>
       <c r="BF121" s="2"/>
       <c r="BG121" s="2"/>
-    </row>
-    <row r="122" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="BH121" s="2"/>
+    </row>
+    <row r="122" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A122" s="2"/>
       <c r="B122" s="2"/>
       <c r="C122" s="2"/>
@@ -29577,8 +29736,9 @@
       <c r="BE122" s="2"/>
       <c r="BF122" s="2"/>
       <c r="BG122" s="2"/>
-    </row>
-    <row r="123" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="BH122" s="2"/>
+    </row>
+    <row r="123" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A123" s="2"/>
       <c r="B123" s="2"/>
       <c r="C123" s="2"/>
@@ -29637,8 +29797,9 @@
       <c r="BE123" s="2"/>
       <c r="BF123" s="2"/>
       <c r="BG123" s="2"/>
-    </row>
-    <row r="124" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="BH123" s="2"/>
+    </row>
+    <row r="124" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A124" s="2"/>
       <c r="B124" s="2"/>
       <c r="C124" s="2"/>
@@ -29697,8 +29858,9 @@
       <c r="BE124" s="2"/>
       <c r="BF124" s="2"/>
       <c r="BG124" s="2"/>
-    </row>
-    <row r="125" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="BH124" s="2"/>
+    </row>
+    <row r="125" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A125" s="2"/>
       <c r="B125" s="2"/>
       <c r="C125" s="2"/>
@@ -29757,8 +29919,9 @@
       <c r="BE125" s="2"/>
       <c r="BF125" s="2"/>
       <c r="BG125" s="2"/>
-    </row>
-    <row r="126" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="BH125" s="2"/>
+    </row>
+    <row r="126" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A126" s="2"/>
       <c r="B126" s="2"/>
       <c r="C126" s="2"/>
@@ -29817,8 +29980,9 @@
       <c r="BE126" s="2"/>
       <c r="BF126" s="2"/>
       <c r="BG126" s="2"/>
-    </row>
-    <row r="127" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="BH126" s="2"/>
+    </row>
+    <row r="127" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A127" s="2"/>
       <c r="B127" s="2"/>
       <c r="C127" s="2"/>
@@ -29877,8 +30041,9 @@
       <c r="BE127" s="2"/>
       <c r="BF127" s="2"/>
       <c r="BG127" s="2"/>
-    </row>
-    <row r="128" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="BH127" s="2"/>
+    </row>
+    <row r="128" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A128" s="2"/>
       <c r="B128" s="2"/>
       <c r="C128" s="2"/>
@@ -29937,8 +30102,9 @@
       <c r="BE128" s="2"/>
       <c r="BF128" s="2"/>
       <c r="BG128" s="2"/>
-    </row>
-    <row r="129" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="BH128" s="2"/>
+    </row>
+    <row r="129" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A129" s="2"/>
       <c r="B129" s="2"/>
       <c r="C129" s="2"/>
@@ -29997,8 +30163,9 @@
       <c r="BE129" s="2"/>
       <c r="BF129" s="2"/>
       <c r="BG129" s="2"/>
-    </row>
-    <row r="130" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="BH129" s="2"/>
+    </row>
+    <row r="130" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A130" s="2"/>
       <c r="B130" s="2"/>
       <c r="C130" s="2"/>
@@ -30057,8 +30224,9 @@
       <c r="BE130" s="2"/>
       <c r="BF130" s="2"/>
       <c r="BG130" s="2"/>
-    </row>
-    <row r="131" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="BH130" s="2"/>
+    </row>
+    <row r="131" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A131" s="2"/>
       <c r="B131" s="2"/>
       <c r="C131" s="2"/>
@@ -30117,8 +30285,9 @@
       <c r="BE131" s="2"/>
       <c r="BF131" s="2"/>
       <c r="BG131" s="2"/>
-    </row>
-    <row r="132" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="BH131" s="2"/>
+    </row>
+    <row r="132" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A132" s="2"/>
       <c r="B132" s="2"/>
       <c r="C132" s="2"/>
@@ -30177,8 +30346,9 @@
       <c r="BE132" s="2"/>
       <c r="BF132" s="2"/>
       <c r="BG132" s="2"/>
-    </row>
-    <row r="133" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="BH132" s="2"/>
+    </row>
+    <row r="133" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A133" s="2"/>
       <c r="B133" s="2"/>
       <c r="C133" s="2"/>
@@ -30237,8 +30407,9 @@
       <c r="BE133" s="2"/>
       <c r="BF133" s="2"/>
       <c r="BG133" s="2"/>
-    </row>
-    <row r="134" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="BH133" s="2"/>
+    </row>
+    <row r="134" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A134" s="2"/>
       <c r="B134" s="2"/>
       <c r="C134" s="2"/>
@@ -30297,8 +30468,9 @@
       <c r="BE134" s="2"/>
       <c r="BF134" s="2"/>
       <c r="BG134" s="2"/>
-    </row>
-    <row r="135" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="BH134" s="2"/>
+    </row>
+    <row r="135" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A135" s="2"/>
       <c r="B135" s="2"/>
       <c r="C135" s="2"/>
@@ -30357,8 +30529,9 @@
       <c r="BE135" s="2"/>
       <c r="BF135" s="2"/>
       <c r="BG135" s="2"/>
-    </row>
-    <row r="136" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="BH135" s="2"/>
+    </row>
+    <row r="136" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A136" s="2"/>
       <c r="B136" s="2"/>
       <c r="C136" s="2"/>
@@ -30417,8 +30590,9 @@
       <c r="BE136" s="2"/>
       <c r="BF136" s="2"/>
       <c r="BG136" s="2"/>
-    </row>
-    <row r="137" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="BH136" s="2"/>
+    </row>
+    <row r="137" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A137" s="2"/>
       <c r="B137" s="2"/>
       <c r="C137" s="2"/>
@@ -30477,8 +30651,9 @@
       <c r="BE137" s="2"/>
       <c r="BF137" s="2"/>
       <c r="BG137" s="2"/>
-    </row>
-    <row r="138" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="BH137" s="2"/>
+    </row>
+    <row r="138" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A138" s="2"/>
       <c r="B138" s="2"/>
       <c r="C138" s="2"/>
@@ -30537,8 +30712,9 @@
       <c r="BE138" s="2"/>
       <c r="BF138" s="2"/>
       <c r="BG138" s="2"/>
-    </row>
-    <row r="139" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="BH138" s="2"/>
+    </row>
+    <row r="139" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A139" s="2"/>
       <c r="B139" s="2"/>
       <c r="C139" s="2"/>
@@ -30597,8 +30773,9 @@
       <c r="BE139" s="2"/>
       <c r="BF139" s="2"/>
       <c r="BG139" s="2"/>
-    </row>
-    <row r="140" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="BH139" s="2"/>
+    </row>
+    <row r="140" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A140" s="2"/>
       <c r="B140" s="2"/>
       <c r="C140" s="2"/>
@@ -30657,8 +30834,9 @@
       <c r="BE140" s="2"/>
       <c r="BF140" s="2"/>
       <c r="BG140" s="2"/>
-    </row>
-    <row r="141" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="BH140" s="2"/>
+    </row>
+    <row r="141" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A141" s="2"/>
       <c r="B141" s="2"/>
       <c r="C141" s="2"/>
@@ -30717,8 +30895,9 @@
       <c r="BE141" s="2"/>
       <c r="BF141" s="2"/>
       <c r="BG141" s="2"/>
-    </row>
-    <row r="142" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="BH141" s="2"/>
+    </row>
+    <row r="142" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A142" s="2"/>
       <c r="B142" s="2"/>
       <c r="C142" s="2"/>
@@ -30777,8 +30956,9 @@
       <c r="BE142" s="2"/>
       <c r="BF142" s="2"/>
       <c r="BG142" s="2"/>
-    </row>
-    <row r="143" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="BH142" s="2"/>
+    </row>
+    <row r="143" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A143" s="2"/>
       <c r="B143" s="2"/>
       <c r="C143" s="2"/>
@@ -30837,8 +31017,9 @@
       <c r="BE143" s="2"/>
       <c r="BF143" s="2"/>
       <c r="BG143" s="2"/>
-    </row>
-    <row r="144" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="BH143" s="2"/>
+    </row>
+    <row r="144" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A144" s="2"/>
       <c r="B144" s="2"/>
       <c r="C144" s="2"/>
@@ -30897,8 +31078,9 @@
       <c r="BE144" s="2"/>
       <c r="BF144" s="2"/>
       <c r="BG144" s="2"/>
-    </row>
-    <row r="145" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="BH144" s="2"/>
+    </row>
+    <row r="145" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A145" s="2"/>
       <c r="B145" s="2"/>
       <c r="C145" s="2"/>
@@ -30957,8 +31139,9 @@
       <c r="BE145" s="2"/>
       <c r="BF145" s="2"/>
       <c r="BG145" s="2"/>
-    </row>
-    <row r="146" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="BH145" s="2"/>
+    </row>
+    <row r="146" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A146" s="2"/>
       <c r="B146" s="2"/>
       <c r="C146" s="2"/>
@@ -31017,8 +31200,9 @@
       <c r="BE146" s="2"/>
       <c r="BF146" s="2"/>
       <c r="BG146" s="2"/>
-    </row>
-    <row r="147" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="BH146" s="2"/>
+    </row>
+    <row r="147" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A147" s="2"/>
       <c r="B147" s="2"/>
       <c r="C147" s="2"/>
@@ -31077,8 +31261,9 @@
       <c r="BE147" s="2"/>
       <c r="BF147" s="2"/>
       <c r="BG147" s="2"/>
-    </row>
-    <row r="148" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="BH147" s="2"/>
+    </row>
+    <row r="148" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A148" s="2"/>
       <c r="B148" s="2"/>
       <c r="C148" s="2"/>
@@ -31137,8 +31322,9 @@
       <c r="BE148" s="2"/>
       <c r="BF148" s="2"/>
       <c r="BG148" s="2"/>
-    </row>
-    <row r="149" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="BH148" s="2"/>
+    </row>
+    <row r="149" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A149" s="2"/>
       <c r="B149" s="2"/>
       <c r="C149" s="2"/>
@@ -31197,8 +31383,9 @@
       <c r="BE149" s="2"/>
       <c r="BF149" s="2"/>
       <c r="BG149" s="2"/>
-    </row>
-    <row r="150" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="BH149" s="2"/>
+    </row>
+    <row r="150" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A150" s="2"/>
       <c r="B150" s="2"/>
       <c r="C150" s="2"/>
@@ -31257,8 +31444,9 @@
       <c r="BE150" s="2"/>
       <c r="BF150" s="2"/>
       <c r="BG150" s="2"/>
-    </row>
-    <row r="151" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="BH150" s="2"/>
+    </row>
+    <row r="151" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A151" s="2"/>
       <c r="B151" s="2"/>
       <c r="C151" s="2"/>
@@ -31317,8 +31505,9 @@
       <c r="BE151" s="2"/>
       <c r="BF151" s="2"/>
       <c r="BG151" s="2"/>
-    </row>
-    <row r="152" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="BH151" s="2"/>
+    </row>
+    <row r="152" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A152" s="2"/>
       <c r="B152" s="2"/>
       <c r="C152" s="2"/>
@@ -31377,8 +31566,9 @@
       <c r="BE152" s="2"/>
       <c r="BF152" s="2"/>
       <c r="BG152" s="2"/>
-    </row>
-    <row r="153" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="BH152" s="2"/>
+    </row>
+    <row r="153" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A153" s="2"/>
       <c r="B153" s="2"/>
       <c r="C153" s="2"/>
@@ -31437,8 +31627,9 @@
       <c r="BE153" s="2"/>
       <c r="BF153" s="2"/>
       <c r="BG153" s="2"/>
-    </row>
-    <row r="154" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="BH153" s="2"/>
+    </row>
+    <row r="154" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A154" s="2"/>
       <c r="B154" s="2"/>
       <c r="C154" s="2"/>
@@ -31497,8 +31688,9 @@
       <c r="BE154" s="2"/>
       <c r="BF154" s="2"/>
       <c r="BG154" s="2"/>
-    </row>
-    <row r="155" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="BH154" s="2"/>
+    </row>
+    <row r="155" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A155" s="2"/>
       <c r="B155" s="2"/>
       <c r="C155" s="2"/>
@@ -31557,8 +31749,9 @@
       <c r="BE155" s="2"/>
       <c r="BF155" s="2"/>
       <c r="BG155" s="2"/>
-    </row>
-    <row r="156" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="BH155" s="2"/>
+    </row>
+    <row r="156" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A156" s="2"/>
       <c r="B156" s="2"/>
       <c r="C156" s="2"/>
@@ -31617,8 +31810,9 @@
       <c r="BE156" s="2"/>
       <c r="BF156" s="2"/>
       <c r="BG156" s="2"/>
-    </row>
-    <row r="157" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="BH156" s="2"/>
+    </row>
+    <row r="157" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A157" s="2"/>
       <c r="B157" s="2"/>
       <c r="C157" s="2"/>
@@ -31677,8 +31871,9 @@
       <c r="BE157" s="2"/>
       <c r="BF157" s="2"/>
       <c r="BG157" s="2"/>
-    </row>
-    <row r="158" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="BH157" s="2"/>
+    </row>
+    <row r="158" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A158" s="2"/>
       <c r="B158" s="2"/>
       <c r="C158" s="2"/>
@@ -31737,8 +31932,9 @@
       <c r="BE158" s="2"/>
       <c r="BF158" s="2"/>
       <c r="BG158" s="2"/>
-    </row>
-    <row r="159" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="BH158" s="2"/>
+    </row>
+    <row r="159" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A159" s="2"/>
       <c r="B159" s="2"/>
       <c r="C159" s="2"/>
@@ -31797,8 +31993,9 @@
       <c r="BE159" s="2"/>
       <c r="BF159" s="2"/>
       <c r="BG159" s="2"/>
-    </row>
-    <row r="160" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="BH159" s="2"/>
+    </row>
+    <row r="160" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A160" s="2"/>
       <c r="B160" s="2"/>
       <c r="C160" s="2"/>
@@ -31857,8 +32054,9 @@
       <c r="BE160" s="2"/>
       <c r="BF160" s="2"/>
       <c r="BG160" s="2"/>
-    </row>
-    <row r="161" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="BH160" s="2"/>
+    </row>
+    <row r="161" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A161" s="2"/>
       <c r="B161" s="2"/>
       <c r="C161" s="2"/>
@@ -31917,8 +32115,9 @@
       <c r="BE161" s="2"/>
       <c r="BF161" s="2"/>
       <c r="BG161" s="2"/>
-    </row>
-    <row r="162" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="BH161" s="2"/>
+    </row>
+    <row r="162" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A162" s="2"/>
       <c r="B162" s="2"/>
       <c r="C162" s="2"/>
@@ -31977,8 +32176,9 @@
       <c r="BE162" s="2"/>
       <c r="BF162" s="2"/>
       <c r="BG162" s="2"/>
-    </row>
-    <row r="163" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="BH162" s="2"/>
+    </row>
+    <row r="163" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A163" s="2"/>
       <c r="B163" s="2"/>
       <c r="C163" s="2"/>
@@ -32037,8 +32237,9 @@
       <c r="BE163" s="2"/>
       <c r="BF163" s="2"/>
       <c r="BG163" s="2"/>
-    </row>
-    <row r="164" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="BH163" s="2"/>
+    </row>
+    <row r="164" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A164" s="2"/>
       <c r="B164" s="2"/>
       <c r="C164" s="2"/>
@@ -32097,8 +32298,9 @@
       <c r="BE164" s="2"/>
       <c r="BF164" s="2"/>
       <c r="BG164" s="2"/>
-    </row>
-    <row r="165" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="BH164" s="2"/>
+    </row>
+    <row r="165" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A165" s="2"/>
       <c r="B165" s="2"/>
       <c r="C165" s="2"/>
@@ -32157,8 +32359,9 @@
       <c r="BE165" s="2"/>
       <c r="BF165" s="2"/>
       <c r="BG165" s="2"/>
-    </row>
-    <row r="166" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="BH165" s="2"/>
+    </row>
+    <row r="166" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A166" s="2"/>
       <c r="B166" s="2"/>
       <c r="C166" s="2"/>
@@ -32217,8 +32420,9 @@
       <c r="BE166" s="2"/>
       <c r="BF166" s="2"/>
       <c r="BG166" s="2"/>
-    </row>
-    <row r="167" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="BH166" s="2"/>
+    </row>
+    <row r="167" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A167" s="2"/>
       <c r="B167" s="2"/>
       <c r="C167" s="2"/>
@@ -32277,8 +32481,9 @@
       <c r="BE167" s="2"/>
       <c r="BF167" s="2"/>
       <c r="BG167" s="2"/>
-    </row>
-    <row r="168" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="BH167" s="2"/>
+    </row>
+    <row r="168" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A168" s="2"/>
       <c r="B168" s="2"/>
       <c r="C168" s="2"/>
@@ -32337,8 +32542,9 @@
       <c r="BE168" s="2"/>
       <c r="BF168" s="2"/>
       <c r="BG168" s="2"/>
-    </row>
-    <row r="169" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="BH168" s="2"/>
+    </row>
+    <row r="169" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A169" s="2"/>
       <c r="B169" s="2"/>
       <c r="C169" s="2"/>
@@ -32397,8 +32603,9 @@
       <c r="BE169" s="2"/>
       <c r="BF169" s="2"/>
       <c r="BG169" s="2"/>
-    </row>
-    <row r="170" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="BH169" s="2"/>
+    </row>
+    <row r="170" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A170" s="2"/>
       <c r="B170" s="2"/>
       <c r="C170" s="2"/>
@@ -32457,8 +32664,9 @@
       <c r="BE170" s="2"/>
       <c r="BF170" s="2"/>
       <c r="BG170" s="2"/>
-    </row>
-    <row r="171" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="BH170" s="2"/>
+    </row>
+    <row r="171" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A171" s="2"/>
       <c r="B171" s="2"/>
       <c r="C171" s="2"/>
@@ -32517,8 +32725,9 @@
       <c r="BE171" s="2"/>
       <c r="BF171" s="2"/>
       <c r="BG171" s="2"/>
-    </row>
-    <row r="172" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="BH171" s="2"/>
+    </row>
+    <row r="172" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A172" s="2"/>
       <c r="B172" s="2"/>
       <c r="C172" s="2"/>
@@ -32577,8 +32786,9 @@
       <c r="BE172" s="2"/>
       <c r="BF172" s="2"/>
       <c r="BG172" s="2"/>
-    </row>
-    <row r="173" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="BH172" s="2"/>
+    </row>
+    <row r="173" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A173" s="2"/>
       <c r="B173" s="2"/>
       <c r="C173" s="2"/>
@@ -32637,8 +32847,9 @@
       <c r="BE173" s="2"/>
       <c r="BF173" s="2"/>
       <c r="BG173" s="2"/>
-    </row>
-    <row r="174" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="BH173" s="2"/>
+    </row>
+    <row r="174" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A174" s="2"/>
       <c r="B174" s="2"/>
       <c r="C174" s="2"/>
@@ -32697,8 +32908,9 @@
       <c r="BE174" s="2"/>
       <c r="BF174" s="2"/>
       <c r="BG174" s="2"/>
-    </row>
-    <row r="175" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="BH174" s="2"/>
+    </row>
+    <row r="175" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A175" s="2"/>
       <c r="B175" s="2"/>
       <c r="C175" s="2"/>
@@ -32757,8 +32969,9 @@
       <c r="BE175" s="2"/>
       <c r="BF175" s="2"/>
       <c r="BG175" s="2"/>
-    </row>
-    <row r="176" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="BH175" s="2"/>
+    </row>
+    <row r="176" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A176" s="2"/>
       <c r="B176" s="2"/>
       <c r="C176" s="2"/>
@@ -32817,8 +33030,9 @@
       <c r="BE176" s="2"/>
       <c r="BF176" s="2"/>
       <c r="BG176" s="2"/>
-    </row>
-    <row r="177" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="BH176" s="2"/>
+    </row>
+    <row r="177" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A177" s="2"/>
       <c r="B177" s="2"/>
       <c r="C177" s="2"/>
@@ -32877,8 +33091,9 @@
       <c r="BE177" s="2"/>
       <c r="BF177" s="2"/>
       <c r="BG177" s="2"/>
-    </row>
-    <row r="178" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="BH177" s="2"/>
+    </row>
+    <row r="178" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A178" s="2"/>
       <c r="B178" s="2"/>
       <c r="C178" s="2"/>
@@ -32937,8 +33152,9 @@
       <c r="BE178" s="2"/>
       <c r="BF178" s="2"/>
       <c r="BG178" s="2"/>
-    </row>
-    <row r="179" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="BH178" s="2"/>
+    </row>
+    <row r="179" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A179" s="2"/>
       <c r="B179" s="2"/>
       <c r="C179" s="2"/>
@@ -32997,8 +33213,9 @@
       <c r="BE179" s="2"/>
       <c r="BF179" s="2"/>
       <c r="BG179" s="2"/>
-    </row>
-    <row r="180" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="BH179" s="2"/>
+    </row>
+    <row r="180" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A180" s="2"/>
       <c r="B180" s="2"/>
       <c r="C180" s="2"/>
@@ -33057,8 +33274,9 @@
       <c r="BE180" s="2"/>
       <c r="BF180" s="2"/>
       <c r="BG180" s="2"/>
-    </row>
-    <row r="181" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="BH180" s="2"/>
+    </row>
+    <row r="181" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A181" s="2"/>
       <c r="B181" s="2"/>
       <c r="C181" s="2"/>
@@ -33117,8 +33335,9 @@
       <c r="BE181" s="2"/>
       <c r="BF181" s="2"/>
       <c r="BG181" s="2"/>
-    </row>
-    <row r="182" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="BH181" s="2"/>
+    </row>
+    <row r="182" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A182" s="2"/>
       <c r="B182" s="2"/>
       <c r="C182" s="2"/>
@@ -33177,8 +33396,9 @@
       <c r="BE182" s="2"/>
       <c r="BF182" s="2"/>
       <c r="BG182" s="2"/>
-    </row>
-    <row r="183" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="BH182" s="2"/>
+    </row>
+    <row r="183" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A183" s="2"/>
       <c r="B183" s="2"/>
       <c r="C183" s="2"/>
@@ -33237,8 +33457,9 @@
       <c r="BE183" s="2"/>
       <c r="BF183" s="2"/>
       <c r="BG183" s="2"/>
-    </row>
-    <row r="184" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="BH183" s="2"/>
+    </row>
+    <row r="184" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A184" s="2"/>
       <c r="B184" s="2"/>
       <c r="C184" s="2"/>
@@ -33297,8 +33518,9 @@
       <c r="BE184" s="2"/>
       <c r="BF184" s="2"/>
       <c r="BG184" s="2"/>
-    </row>
-    <row r="185" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="BH184" s="2"/>
+    </row>
+    <row r="185" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A185" s="2"/>
       <c r="B185" s="2"/>
       <c r="C185" s="2"/>
@@ -33357,8 +33579,9 @@
       <c r="BE185" s="2"/>
       <c r="BF185" s="2"/>
       <c r="BG185" s="2"/>
-    </row>
-    <row r="186" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="BH185" s="2"/>
+    </row>
+    <row r="186" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A186" s="2"/>
       <c r="B186" s="2"/>
       <c r="C186" s="2"/>
@@ -33417,8 +33640,9 @@
       <c r="BE186" s="2"/>
       <c r="BF186" s="2"/>
       <c r="BG186" s="2"/>
-    </row>
-    <row r="187" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="BH186" s="2"/>
+    </row>
+    <row r="187" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A187" s="2"/>
       <c r="B187" s="2"/>
       <c r="C187" s="2"/>
@@ -33477,8 +33701,9 @@
       <c r="BE187" s="2"/>
       <c r="BF187" s="2"/>
       <c r="BG187" s="2"/>
-    </row>
-    <row r="188" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="BH187" s="2"/>
+    </row>
+    <row r="188" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A188" s="2"/>
       <c r="B188" s="2"/>
       <c r="C188" s="2"/>
@@ -33537,8 +33762,9 @@
       <c r="BE188" s="2"/>
       <c r="BF188" s="2"/>
       <c r="BG188" s="2"/>
-    </row>
-    <row r="189" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="BH188" s="2"/>
+    </row>
+    <row r="189" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A189" s="2"/>
       <c r="B189" s="2"/>
       <c r="C189" s="2"/>
@@ -33597,8 +33823,9 @@
       <c r="BE189" s="2"/>
       <c r="BF189" s="2"/>
       <c r="BG189" s="2"/>
-    </row>
-    <row r="190" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="BH189" s="2"/>
+    </row>
+    <row r="190" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A190" s="2"/>
       <c r="B190" s="2"/>
       <c r="C190" s="2"/>
@@ -33657,8 +33884,9 @@
       <c r="BE190" s="2"/>
       <c r="BF190" s="2"/>
       <c r="BG190" s="2"/>
-    </row>
-    <row r="191" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="BH190" s="2"/>
+    </row>
+    <row r="191" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A191" s="2"/>
       <c r="B191" s="2"/>
       <c r="C191" s="2"/>
@@ -33717,8 +33945,9 @@
       <c r="BE191" s="2"/>
       <c r="BF191" s="2"/>
       <c r="BG191" s="2"/>
-    </row>
-    <row r="192" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="BH191" s="2"/>
+    </row>
+    <row r="192" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A192" s="2"/>
       <c r="B192" s="2"/>
       <c r="C192" s="2"/>
@@ -33777,8 +34006,9 @@
       <c r="BE192" s="2"/>
       <c r="BF192" s="2"/>
       <c r="BG192" s="2"/>
-    </row>
-    <row r="193" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="BH192" s="2"/>
+    </row>
+    <row r="193" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A193" s="2"/>
       <c r="B193" s="2"/>
       <c r="C193" s="2"/>
@@ -33837,8 +34067,9 @@
       <c r="BE193" s="2"/>
       <c r="BF193" s="2"/>
       <c r="BG193" s="2"/>
-    </row>
-    <row r="194" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="BH193" s="2"/>
+    </row>
+    <row r="194" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A194" s="2"/>
       <c r="B194" s="2"/>
       <c r="C194" s="2"/>
@@ -33897,8 +34128,9 @@
       <c r="BE194" s="2"/>
       <c r="BF194" s="2"/>
       <c r="BG194" s="2"/>
-    </row>
-    <row r="195" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="BH194" s="2"/>
+    </row>
+    <row r="195" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A195" s="2"/>
       <c r="B195" s="2"/>
       <c r="C195" s="2"/>
@@ -33957,8 +34189,9 @@
       <c r="BE195" s="2"/>
       <c r="BF195" s="2"/>
       <c r="BG195" s="2"/>
-    </row>
-    <row r="196" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="BH195" s="2"/>
+    </row>
+    <row r="196" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A196" s="2"/>
       <c r="B196" s="2"/>
       <c r="C196" s="2"/>
@@ -34017,8 +34250,9 @@
       <c r="BE196" s="2"/>
       <c r="BF196" s="2"/>
       <c r="BG196" s="2"/>
-    </row>
-    <row r="197" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="BH196" s="2"/>
+    </row>
+    <row r="197" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A197" s="2"/>
       <c r="B197" s="2"/>
       <c r="C197" s="2"/>
@@ -34077,8 +34311,9 @@
       <c r="BE197" s="2"/>
       <c r="BF197" s="2"/>
       <c r="BG197" s="2"/>
-    </row>
-    <row r="198" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="BH197" s="2"/>
+    </row>
+    <row r="198" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A198" s="2"/>
       <c r="B198" s="2"/>
       <c r="C198" s="2"/>
@@ -34137,8 +34372,9 @@
       <c r="BE198" s="2"/>
       <c r="BF198" s="2"/>
       <c r="BG198" s="2"/>
-    </row>
-    <row r="199" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="BH198" s="2"/>
+    </row>
+    <row r="199" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A199" s="2"/>
       <c r="B199" s="2"/>
       <c r="C199" s="2"/>
@@ -34197,8 +34433,9 @@
       <c r="BE199" s="2"/>
       <c r="BF199" s="2"/>
       <c r="BG199" s="2"/>
-    </row>
-    <row r="200" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="BH199" s="2"/>
+    </row>
+    <row r="200" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A200" s="2"/>
       <c r="B200" s="2"/>
       <c r="C200" s="2"/>
@@ -34257,8 +34494,9 @@
       <c r="BE200" s="2"/>
       <c r="BF200" s="2"/>
       <c r="BG200" s="2"/>
-    </row>
-    <row r="201" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="BH200" s="2"/>
+    </row>
+    <row r="201" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A201" s="2"/>
       <c r="B201" s="2"/>
       <c r="C201" s="2"/>
@@ -34317,8 +34555,9 @@
       <c r="BE201" s="2"/>
       <c r="BF201" s="2"/>
       <c r="BG201" s="2"/>
-    </row>
-    <row r="202" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="BH201" s="2"/>
+    </row>
+    <row r="202" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A202" s="2"/>
       <c r="B202" s="2"/>
       <c r="C202" s="2"/>
@@ -34377,8 +34616,9 @@
       <c r="BE202" s="2"/>
       <c r="BF202" s="2"/>
       <c r="BG202" s="2"/>
-    </row>
-    <row r="203" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="BH202" s="2"/>
+    </row>
+    <row r="203" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A203" s="2"/>
       <c r="B203" s="2"/>
       <c r="C203" s="2"/>
@@ -34437,8 +34677,9 @@
       <c r="BE203" s="2"/>
       <c r="BF203" s="2"/>
       <c r="BG203" s="2"/>
-    </row>
-    <row r="204" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="BH203" s="2"/>
+    </row>
+    <row r="204" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A204" s="2"/>
       <c r="B204" s="2"/>
       <c r="C204" s="2"/>
@@ -34497,8 +34738,9 @@
       <c r="BE204" s="2"/>
       <c r="BF204" s="2"/>
       <c r="BG204" s="2"/>
-    </row>
-    <row r="205" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="BH204" s="2"/>
+    </row>
+    <row r="205" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A205" s="2"/>
       <c r="B205" s="2"/>
       <c r="C205" s="2"/>
@@ -34557,8 +34799,9 @@
       <c r="BE205" s="2"/>
       <c r="BF205" s="2"/>
       <c r="BG205" s="2"/>
-    </row>
-    <row r="206" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="BH205" s="2"/>
+    </row>
+    <row r="206" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A206" s="2"/>
       <c r="B206" s="2"/>
       <c r="C206" s="2"/>
@@ -34617,8 +34860,9 @@
       <c r="BE206" s="2"/>
       <c r="BF206" s="2"/>
       <c r="BG206" s="2"/>
-    </row>
-    <row r="207" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="BH206" s="2"/>
+    </row>
+    <row r="207" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A207" s="2"/>
       <c r="B207" s="2"/>
       <c r="C207" s="2"/>
@@ -34677,8 +34921,9 @@
       <c r="BE207" s="2"/>
       <c r="BF207" s="2"/>
       <c r="BG207" s="2"/>
-    </row>
-    <row r="208" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="BH207" s="2"/>
+    </row>
+    <row r="208" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A208" s="2"/>
       <c r="B208" s="2"/>
       <c r="C208" s="2"/>
@@ -34737,8 +34982,9 @@
       <c r="BE208" s="2"/>
       <c r="BF208" s="2"/>
       <c r="BG208" s="2"/>
-    </row>
-    <row r="209" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="BH208" s="2"/>
+    </row>
+    <row r="209" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A209" s="2"/>
       <c r="B209" s="2"/>
       <c r="C209" s="2"/>
@@ -34797,8 +35043,9 @@
       <c r="BE209" s="2"/>
       <c r="BF209" s="2"/>
       <c r="BG209" s="2"/>
-    </row>
-    <row r="210" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="BH209" s="2"/>
+    </row>
+    <row r="210" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A210" s="2"/>
       <c r="B210" s="2"/>
       <c r="C210" s="2"/>
@@ -34857,8 +35104,9 @@
       <c r="BE210" s="2"/>
       <c r="BF210" s="2"/>
       <c r="BG210" s="2"/>
-    </row>
-    <row r="211" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="BH210" s="2"/>
+    </row>
+    <row r="211" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A211" s="2"/>
       <c r="B211" s="2"/>
       <c r="C211" s="2"/>
@@ -34917,8 +35165,9 @@
       <c r="BE211" s="2"/>
       <c r="BF211" s="2"/>
       <c r="BG211" s="2"/>
-    </row>
-    <row r="212" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="BH211" s="2"/>
+    </row>
+    <row r="212" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A212" s="2"/>
       <c r="B212" s="2"/>
       <c r="C212" s="2"/>
@@ -34977,8 +35226,9 @@
       <c r="BE212" s="2"/>
       <c r="BF212" s="2"/>
       <c r="BG212" s="2"/>
-    </row>
-    <row r="213" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="BH212" s="2"/>
+    </row>
+    <row r="213" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A213" s="2"/>
       <c r="B213" s="2"/>
       <c r="C213" s="2"/>
@@ -35037,8 +35287,9 @@
       <c r="BE213" s="2"/>
       <c r="BF213" s="2"/>
       <c r="BG213" s="2"/>
-    </row>
-    <row r="214" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="BH213" s="2"/>
+    </row>
+    <row r="214" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A214" s="2"/>
       <c r="B214" s="2"/>
       <c r="C214" s="2"/>
@@ -35097,8 +35348,9 @@
       <c r="BE214" s="2"/>
       <c r="BF214" s="2"/>
       <c r="BG214" s="2"/>
-    </row>
-    <row r="215" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="BH214" s="2"/>
+    </row>
+    <row r="215" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A215" s="2"/>
       <c r="B215" s="2"/>
       <c r="C215" s="2"/>
@@ -35157,8 +35409,9 @@
       <c r="BE215" s="2"/>
       <c r="BF215" s="2"/>
       <c r="BG215" s="2"/>
-    </row>
-    <row r="216" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="BH215" s="2"/>
+    </row>
+    <row r="216" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A216" s="2"/>
       <c r="B216" s="2"/>
       <c r="C216" s="2"/>
@@ -35217,8 +35470,9 @@
       <c r="BE216" s="2"/>
       <c r="BF216" s="2"/>
       <c r="BG216" s="2"/>
-    </row>
-    <row r="217" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="BH216" s="2"/>
+    </row>
+    <row r="217" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A217" s="2"/>
       <c r="B217" s="2"/>
       <c r="C217" s="2"/>
@@ -35277,8 +35531,9 @@
       <c r="BE217" s="2"/>
       <c r="BF217" s="2"/>
       <c r="BG217" s="2"/>
-    </row>
-    <row r="218" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="BH217" s="2"/>
+    </row>
+    <row r="218" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A218" s="2"/>
       <c r="B218" s="2"/>
       <c r="C218" s="2"/>
@@ -35337,8 +35592,9 @@
       <c r="BE218" s="2"/>
       <c r="BF218" s="2"/>
       <c r="BG218" s="2"/>
-    </row>
-    <row r="219" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="BH218" s="2"/>
+    </row>
+    <row r="219" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A219" s="2"/>
       <c r="B219" s="2"/>
       <c r="C219" s="2"/>
@@ -35397,8 +35653,9 @@
       <c r="BE219" s="2"/>
       <c r="BF219" s="2"/>
       <c r="BG219" s="2"/>
-    </row>
-    <row r="220" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="BH219" s="2"/>
+    </row>
+    <row r="220" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A220" s="2"/>
       <c r="B220" s="2"/>
       <c r="C220" s="2"/>
@@ -35457,8 +35714,9 @@
       <c r="BE220" s="2"/>
       <c r="BF220" s="2"/>
       <c r="BG220" s="2"/>
-    </row>
-    <row r="221" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="BH220" s="2"/>
+    </row>
+    <row r="221" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A221" s="2"/>
       <c r="B221" s="2"/>
       <c r="C221" s="2"/>
@@ -35517,8 +35775,9 @@
       <c r="BE221" s="2"/>
       <c r="BF221" s="2"/>
       <c r="BG221" s="2"/>
-    </row>
-    <row r="222" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="BH221" s="2"/>
+    </row>
+    <row r="222" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A222" s="2"/>
       <c r="B222" s="2"/>
       <c r="C222" s="2"/>
@@ -35577,8 +35836,9 @@
       <c r="BE222" s="2"/>
       <c r="BF222" s="2"/>
       <c r="BG222" s="2"/>
-    </row>
-    <row r="223" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="BH222" s="2"/>
+    </row>
+    <row r="223" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A223" s="2"/>
       <c r="B223" s="2"/>
       <c r="C223" s="2"/>
@@ -35637,8 +35897,9 @@
       <c r="BE223" s="2"/>
       <c r="BF223" s="2"/>
       <c r="BG223" s="2"/>
-    </row>
-    <row r="224" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="BH223" s="2"/>
+    </row>
+    <row r="224" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A224" s="2"/>
       <c r="B224" s="2"/>
       <c r="C224" s="2"/>
@@ -35697,8 +35958,9 @@
       <c r="BE224" s="2"/>
       <c r="BF224" s="2"/>
       <c r="BG224" s="2"/>
-    </row>
-    <row r="225" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="BH224" s="2"/>
+    </row>
+    <row r="225" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A225" s="2"/>
       <c r="B225" s="2"/>
       <c r="C225" s="2"/>
@@ -35757,8 +36019,9 @@
       <c r="BE225" s="2"/>
       <c r="BF225" s="2"/>
       <c r="BG225" s="2"/>
-    </row>
-    <row r="226" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="BH225" s="2"/>
+    </row>
+    <row r="226" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A226" s="2"/>
       <c r="B226" s="2"/>
       <c r="C226" s="2"/>
@@ -35817,8 +36080,9 @@
       <c r="BE226" s="2"/>
       <c r="BF226" s="2"/>
       <c r="BG226" s="2"/>
-    </row>
-    <row r="227" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="BH226" s="2"/>
+    </row>
+    <row r="227" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A227" s="2"/>
       <c r="B227" s="2"/>
       <c r="C227" s="2"/>
@@ -35877,8 +36141,9 @@
       <c r="BE227" s="2"/>
       <c r="BF227" s="2"/>
       <c r="BG227" s="2"/>
-    </row>
-    <row r="228" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="BH227" s="2"/>
+    </row>
+    <row r="228" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A228" s="2"/>
       <c r="B228" s="2"/>
       <c r="C228" s="2"/>
@@ -35937,8 +36202,9 @@
       <c r="BE228" s="2"/>
       <c r="BF228" s="2"/>
       <c r="BG228" s="2"/>
-    </row>
-    <row r="229" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="BH228" s="2"/>
+    </row>
+    <row r="229" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A229" s="2"/>
       <c r="B229" s="2"/>
       <c r="C229" s="2"/>
@@ -35997,8 +36263,9 @@
       <c r="BE229" s="2"/>
       <c r="BF229" s="2"/>
       <c r="BG229" s="2"/>
-    </row>
-    <row r="230" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="BH229" s="2"/>
+    </row>
+    <row r="230" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A230" s="2"/>
       <c r="B230" s="2"/>
       <c r="C230" s="2"/>
@@ -36057,8 +36324,9 @@
       <c r="BE230" s="2"/>
       <c r="BF230" s="2"/>
       <c r="BG230" s="2"/>
-    </row>
-    <row r="231" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="BH230" s="2"/>
+    </row>
+    <row r="231" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A231" s="2"/>
       <c r="B231" s="2"/>
       <c r="C231" s="2"/>
@@ -36117,8 +36385,9 @@
       <c r="BE231" s="2"/>
       <c r="BF231" s="2"/>
       <c r="BG231" s="2"/>
-    </row>
-    <row r="232" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="BH231" s="2"/>
+    </row>
+    <row r="232" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A232" s="2"/>
       <c r="B232" s="2"/>
       <c r="C232" s="2"/>
@@ -36177,8 +36446,9 @@
       <c r="BE232" s="2"/>
       <c r="BF232" s="2"/>
       <c r="BG232" s="2"/>
-    </row>
-    <row r="233" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="BH232" s="2"/>
+    </row>
+    <row r="233" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A233" s="2"/>
       <c r="B233" s="2"/>
       <c r="C233" s="2"/>
@@ -36237,8 +36507,9 @@
       <c r="BE233" s="2"/>
       <c r="BF233" s="2"/>
       <c r="BG233" s="2"/>
-    </row>
-    <row r="234" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="BH233" s="2"/>
+    </row>
+    <row r="234" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A234" s="2"/>
       <c r="B234" s="2"/>
       <c r="C234" s="2"/>
@@ -36297,8 +36568,9 @@
       <c r="BE234" s="2"/>
       <c r="BF234" s="2"/>
       <c r="BG234" s="2"/>
-    </row>
-    <row r="235" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="BH234" s="2"/>
+    </row>
+    <row r="235" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A235" s="2"/>
       <c r="B235" s="2"/>
       <c r="C235" s="2"/>
@@ -36357,8 +36629,9 @@
       <c r="BE235" s="2"/>
       <c r="BF235" s="2"/>
       <c r="BG235" s="2"/>
-    </row>
-    <row r="236" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="BH235" s="2"/>
+    </row>
+    <row r="236" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A236" s="2"/>
       <c r="B236" s="2"/>
       <c r="C236" s="2"/>
@@ -36417,8 +36690,9 @@
       <c r="BE236" s="2"/>
       <c r="BF236" s="2"/>
       <c r="BG236" s="2"/>
-    </row>
-    <row r="237" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="BH236" s="2"/>
+    </row>
+    <row r="237" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A237" s="2"/>
       <c r="B237" s="2"/>
       <c r="C237" s="2"/>
@@ -36477,8 +36751,9 @@
       <c r="BE237" s="2"/>
       <c r="BF237" s="2"/>
       <c r="BG237" s="2"/>
-    </row>
-    <row r="238" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="BH237" s="2"/>
+    </row>
+    <row r="238" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A238" s="2"/>
       <c r="B238" s="2"/>
       <c r="C238" s="2"/>
@@ -36537,8 +36812,9 @@
       <c r="BE238" s="2"/>
       <c r="BF238" s="2"/>
       <c r="BG238" s="2"/>
-    </row>
-    <row r="239" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="BH238" s="2"/>
+    </row>
+    <row r="239" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A239" s="2"/>
       <c r="B239" s="2"/>
       <c r="C239" s="2"/>
@@ -36597,8 +36873,9 @@
       <c r="BE239" s="2"/>
       <c r="BF239" s="2"/>
       <c r="BG239" s="2"/>
-    </row>
-    <row r="240" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="BH239" s="2"/>
+    </row>
+    <row r="240" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A240" s="2"/>
       <c r="B240" s="2"/>
       <c r="C240" s="2"/>
@@ -36657,8 +36934,9 @@
       <c r="BE240" s="2"/>
       <c r="BF240" s="2"/>
       <c r="BG240" s="2"/>
-    </row>
-    <row r="241" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="BH240" s="2"/>
+    </row>
+    <row r="241" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A241" s="2"/>
       <c r="B241" s="2"/>
       <c r="C241" s="2"/>
@@ -36717,8 +36995,9 @@
       <c r="BE241" s="2"/>
       <c r="BF241" s="2"/>
       <c r="BG241" s="2"/>
-    </row>
-    <row r="242" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="BH241" s="2"/>
+    </row>
+    <row r="242" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A242" s="2"/>
       <c r="B242" s="2"/>
       <c r="C242" s="2"/>
@@ -36777,8 +37056,9 @@
       <c r="BE242" s="2"/>
       <c r="BF242" s="2"/>
       <c r="BG242" s="2"/>
-    </row>
-    <row r="243" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="BH242" s="2"/>
+    </row>
+    <row r="243" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A243" s="2"/>
       <c r="B243" s="2"/>
       <c r="C243" s="2"/>
@@ -36837,8 +37117,9 @@
       <c r="BE243" s="2"/>
       <c r="BF243" s="2"/>
       <c r="BG243" s="2"/>
-    </row>
-    <row r="244" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="BH243" s="2"/>
+    </row>
+    <row r="244" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A244" s="2"/>
       <c r="B244" s="2"/>
       <c r="C244" s="2"/>
@@ -36897,8 +37178,9 @@
       <c r="BE244" s="2"/>
       <c r="BF244" s="2"/>
       <c r="BG244" s="2"/>
-    </row>
-    <row r="245" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="BH244" s="2"/>
+    </row>
+    <row r="245" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A245" s="2"/>
       <c r="B245" s="2"/>
       <c r="C245" s="2"/>
@@ -36957,8 +37239,9 @@
       <c r="BE245" s="2"/>
       <c r="BF245" s="2"/>
       <c r="BG245" s="2"/>
-    </row>
-    <row r="246" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="BH245" s="2"/>
+    </row>
+    <row r="246" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A246" s="2"/>
       <c r="B246" s="2"/>
       <c r="C246" s="2"/>
@@ -37017,8 +37300,9 @@
       <c r="BE246" s="2"/>
       <c r="BF246" s="2"/>
       <c r="BG246" s="2"/>
-    </row>
-    <row r="247" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="BH246" s="2"/>
+    </row>
+    <row r="247" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A247" s="2"/>
       <c r="B247" s="2"/>
       <c r="C247" s="2"/>
@@ -37077,8 +37361,9 @@
       <c r="BE247" s="2"/>
       <c r="BF247" s="2"/>
       <c r="BG247" s="2"/>
-    </row>
-    <row r="248" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="BH247" s="2"/>
+    </row>
+    <row r="248" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A248" s="2"/>
       <c r="B248" s="2"/>
       <c r="C248" s="2"/>
@@ -37137,8 +37422,9 @@
       <c r="BE248" s="2"/>
       <c r="BF248" s="2"/>
       <c r="BG248" s="2"/>
-    </row>
-    <row r="249" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="BH248" s="2"/>
+    </row>
+    <row r="249" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A249" s="2"/>
       <c r="B249" s="2"/>
       <c r="C249" s="2"/>
@@ -37197,8 +37483,9 @@
       <c r="BE249" s="2"/>
       <c r="BF249" s="2"/>
       <c r="BG249" s="2"/>
-    </row>
-    <row r="250" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="BH249" s="2"/>
+    </row>
+    <row r="250" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A250" s="2"/>
       <c r="B250" s="2"/>
       <c r="C250" s="2"/>
@@ -37257,8 +37544,9 @@
       <c r="BE250" s="2"/>
       <c r="BF250" s="2"/>
       <c r="BG250" s="2"/>
-    </row>
-    <row r="251" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="BH250" s="2"/>
+    </row>
+    <row r="251" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A251" s="2"/>
       <c r="B251" s="2"/>
       <c r="C251" s="2"/>
@@ -37317,8 +37605,9 @@
       <c r="BE251" s="2"/>
       <c r="BF251" s="2"/>
       <c r="BG251" s="2"/>
-    </row>
-    <row r="252" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="BH251" s="2"/>
+    </row>
+    <row r="252" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A252" s="2"/>
       <c r="B252" s="2"/>
       <c r="C252" s="2"/>
@@ -37377,8 +37666,9 @@
       <c r="BE252" s="2"/>
       <c r="BF252" s="2"/>
       <c r="BG252" s="2"/>
-    </row>
-    <row r="253" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="BH252" s="2"/>
+    </row>
+    <row r="253" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A253" s="2"/>
       <c r="B253" s="2"/>
       <c r="C253" s="2"/>
@@ -37437,8 +37727,9 @@
       <c r="BE253" s="2"/>
       <c r="BF253" s="2"/>
       <c r="BG253" s="2"/>
-    </row>
-    <row r="254" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="BH253" s="2"/>
+    </row>
+    <row r="254" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A254" s="2"/>
       <c r="B254" s="2"/>
       <c r="C254" s="2"/>
@@ -37497,8 +37788,9 @@
       <c r="BE254" s="2"/>
       <c r="BF254" s="2"/>
       <c r="BG254" s="2"/>
-    </row>
-    <row r="255" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="BH254" s="2"/>
+    </row>
+    <row r="255" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A255" s="2"/>
       <c r="B255" s="2"/>
       <c r="C255" s="2"/>
@@ -37557,8 +37849,9 @@
       <c r="BE255" s="2"/>
       <c r="BF255" s="2"/>
       <c r="BG255" s="2"/>
-    </row>
-    <row r="256" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="BH255" s="2"/>
+    </row>
+    <row r="256" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A256" s="2"/>
       <c r="B256" s="2"/>
       <c r="C256" s="2"/>
@@ -37617,8 +37910,9 @@
       <c r="BE256" s="2"/>
       <c r="BF256" s="2"/>
       <c r="BG256" s="2"/>
-    </row>
-    <row r="257" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="BH256" s="2"/>
+    </row>
+    <row r="257" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A257" s="2"/>
       <c r="B257" s="2"/>
       <c r="C257" s="2"/>
@@ -37677,8 +37971,9 @@
       <c r="BE257" s="2"/>
       <c r="BF257" s="2"/>
       <c r="BG257" s="2"/>
-    </row>
-    <row r="258" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="BH257" s="2"/>
+    </row>
+    <row r="258" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A258" s="2"/>
       <c r="B258" s="2"/>
       <c r="C258" s="2"/>
@@ -37737,8 +38032,9 @@
       <c r="BE258" s="2"/>
       <c r="BF258" s="2"/>
       <c r="BG258" s="2"/>
-    </row>
-    <row r="259" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="BH258" s="2"/>
+    </row>
+    <row r="259" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A259" s="2"/>
       <c r="B259" s="2"/>
       <c r="C259" s="2"/>
@@ -37797,8 +38093,9 @@
       <c r="BE259" s="2"/>
       <c r="BF259" s="2"/>
       <c r="BG259" s="2"/>
-    </row>
-    <row r="260" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="BH259" s="2"/>
+    </row>
+    <row r="260" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A260" s="2"/>
       <c r="B260" s="2"/>
       <c r="C260" s="2"/>
@@ -37857,8 +38154,9 @@
       <c r="BE260" s="2"/>
       <c r="BF260" s="2"/>
       <c r="BG260" s="2"/>
-    </row>
-    <row r="261" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="BH260" s="2"/>
+    </row>
+    <row r="261" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A261" s="2"/>
       <c r="B261" s="2"/>
       <c r="C261" s="2"/>
@@ -37917,8 +38215,9 @@
       <c r="BE261" s="2"/>
       <c r="BF261" s="2"/>
       <c r="BG261" s="2"/>
-    </row>
-    <row r="262" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="BH261" s="2"/>
+    </row>
+    <row r="262" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A262" s="2"/>
       <c r="B262" s="2"/>
       <c r="C262" s="2"/>
@@ -37977,8 +38276,9 @@
       <c r="BE262" s="2"/>
       <c r="BF262" s="2"/>
       <c r="BG262" s="2"/>
-    </row>
-    <row r="263" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="BH262" s="2"/>
+    </row>
+    <row r="263" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A263" s="2"/>
       <c r="B263" s="2"/>
       <c r="C263" s="2"/>
@@ -38037,8 +38337,9 @@
       <c r="BE263" s="2"/>
       <c r="BF263" s="2"/>
       <c r="BG263" s="2"/>
-    </row>
-    <row r="264" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="BH263" s="2"/>
+    </row>
+    <row r="264" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A264" s="2"/>
       <c r="B264" s="2"/>
       <c r="C264" s="2"/>
@@ -38097,8 +38398,9 @@
       <c r="BE264" s="2"/>
       <c r="BF264" s="2"/>
       <c r="BG264" s="2"/>
-    </row>
-    <row r="265" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="BH264" s="2"/>
+    </row>
+    <row r="265" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A265" s="2"/>
       <c r="B265" s="2"/>
       <c r="C265" s="2"/>
@@ -38157,8 +38459,9 @@
       <c r="BE265" s="2"/>
       <c r="BF265" s="2"/>
       <c r="BG265" s="2"/>
-    </row>
-    <row r="266" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="BH265" s="2"/>
+    </row>
+    <row r="266" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A266" s="2"/>
       <c r="B266" s="2"/>
       <c r="C266" s="2"/>
@@ -38217,8 +38520,9 @@
       <c r="BE266" s="2"/>
       <c r="BF266" s="2"/>
       <c r="BG266" s="2"/>
-    </row>
-    <row r="267" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="BH266" s="2"/>
+    </row>
+    <row r="267" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A267" s="2"/>
       <c r="B267" s="2"/>
       <c r="C267" s="2"/>
@@ -38277,8 +38581,9 @@
       <c r="BE267" s="2"/>
       <c r="BF267" s="2"/>
       <c r="BG267" s="2"/>
-    </row>
-    <row r="268" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="BH267" s="2"/>
+    </row>
+    <row r="268" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A268" s="2"/>
       <c r="B268" s="2"/>
       <c r="C268" s="2"/>
@@ -38337,8 +38642,9 @@
       <c r="BE268" s="2"/>
       <c r="BF268" s="2"/>
       <c r="BG268" s="2"/>
-    </row>
-    <row r="269" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="BH268" s="2"/>
+    </row>
+    <row r="269" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A269" s="2"/>
       <c r="B269" s="2"/>
       <c r="C269" s="2"/>
@@ -38397,8 +38703,9 @@
       <c r="BE269" s="2"/>
       <c r="BF269" s="2"/>
       <c r="BG269" s="2"/>
-    </row>
-    <row r="270" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="BH269" s="2"/>
+    </row>
+    <row r="270" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A270" s="2"/>
       <c r="B270" s="2"/>
       <c r="C270" s="2"/>
@@ -38457,8 +38764,9 @@
       <c r="BE270" s="2"/>
       <c r="BF270" s="2"/>
       <c r="BG270" s="2"/>
-    </row>
-    <row r="271" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="BH270" s="2"/>
+    </row>
+    <row r="271" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A271" s="2"/>
       <c r="B271" s="2"/>
       <c r="C271" s="2"/>
@@ -38517,8 +38825,9 @@
       <c r="BE271" s="2"/>
       <c r="BF271" s="2"/>
       <c r="BG271" s="2"/>
-    </row>
-    <row r="272" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="BH271" s="2"/>
+    </row>
+    <row r="272" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A272" s="2"/>
       <c r="B272" s="2"/>
       <c r="C272" s="2"/>
@@ -38577,8 +38886,9 @@
       <c r="BE272" s="2"/>
       <c r="BF272" s="2"/>
       <c r="BG272" s="2"/>
-    </row>
-    <row r="273" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="BH272" s="2"/>
+    </row>
+    <row r="273" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A273" s="2"/>
       <c r="B273" s="2"/>
       <c r="C273" s="2"/>
@@ -38637,8 +38947,9 @@
       <c r="BE273" s="2"/>
       <c r="BF273" s="2"/>
       <c r="BG273" s="2"/>
-    </row>
-    <row r="274" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="BH273" s="2"/>
+    </row>
+    <row r="274" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A274" s="2"/>
       <c r="B274" s="2"/>
       <c r="C274" s="2"/>
@@ -38697,8 +39008,9 @@
       <c r="BE274" s="2"/>
       <c r="BF274" s="2"/>
       <c r="BG274" s="2"/>
-    </row>
-    <row r="275" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="BH274" s="2"/>
+    </row>
+    <row r="275" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A275" s="2"/>
       <c r="B275" s="2"/>
       <c r="C275" s="2"/>
@@ -38757,8 +39069,9 @@
       <c r="BE275" s="2"/>
       <c r="BF275" s="2"/>
       <c r="BG275" s="2"/>
-    </row>
-    <row r="276" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="BH275" s="2"/>
+    </row>
+    <row r="276" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A276" s="2"/>
       <c r="B276" s="2"/>
       <c r="C276" s="2"/>
@@ -38817,8 +39130,9 @@
       <c r="BE276" s="2"/>
       <c r="BF276" s="2"/>
       <c r="BG276" s="2"/>
-    </row>
-    <row r="277" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="BH276" s="2"/>
+    </row>
+    <row r="277" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A277" s="2"/>
       <c r="B277" s="2"/>
       <c r="C277" s="2"/>
@@ -38877,8 +39191,9 @@
       <c r="BE277" s="2"/>
       <c r="BF277" s="2"/>
       <c r="BG277" s="2"/>
-    </row>
-    <row r="278" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="BH277" s="2"/>
+    </row>
+    <row r="278" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A278" s="2"/>
       <c r="B278" s="2"/>
       <c r="C278" s="2"/>
@@ -38937,8 +39252,9 @@
       <c r="BE278" s="2"/>
       <c r="BF278" s="2"/>
       <c r="BG278" s="2"/>
-    </row>
-    <row r="279" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="BH278" s="2"/>
+    </row>
+    <row r="279" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A279" s="2"/>
       <c r="B279" s="2"/>
       <c r="C279" s="2"/>
@@ -38997,8 +39313,9 @@
       <c r="BE279" s="2"/>
       <c r="BF279" s="2"/>
       <c r="BG279" s="2"/>
-    </row>
-    <row r="280" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="BH279" s="2"/>
+    </row>
+    <row r="280" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A280" s="2"/>
       <c r="B280" s="2"/>
       <c r="C280" s="2"/>
@@ -39057,8 +39374,9 @@
       <c r="BE280" s="2"/>
       <c r="BF280" s="2"/>
       <c r="BG280" s="2"/>
-    </row>
-    <row r="281" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="BH280" s="2"/>
+    </row>
+    <row r="281" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A281" s="2"/>
       <c r="B281" s="2"/>
       <c r="C281" s="2"/>
@@ -39117,8 +39435,9 @@
       <c r="BE281" s="2"/>
       <c r="BF281" s="2"/>
       <c r="BG281" s="2"/>
-    </row>
-    <row r="282" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="BH281" s="2"/>
+    </row>
+    <row r="282" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A282" s="2"/>
       <c r="B282" s="2"/>
       <c r="C282" s="2"/>
@@ -39177,8 +39496,9 @@
       <c r="BE282" s="2"/>
       <c r="BF282" s="2"/>
       <c r="BG282" s="2"/>
-    </row>
-    <row r="283" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="BH282" s="2"/>
+    </row>
+    <row r="283" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A283" s="2"/>
       <c r="B283" s="2"/>
       <c r="C283" s="2"/>
@@ -39237,8 +39557,9 @@
       <c r="BE283" s="2"/>
       <c r="BF283" s="2"/>
       <c r="BG283" s="2"/>
-    </row>
-    <row r="284" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="BH283" s="2"/>
+    </row>
+    <row r="284" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A284" s="2"/>
       <c r="B284" s="2"/>
       <c r="C284" s="2"/>
@@ -39297,8 +39618,9 @@
       <c r="BE284" s="2"/>
       <c r="BF284" s="2"/>
       <c r="BG284" s="2"/>
-    </row>
-    <row r="285" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="BH284" s="2"/>
+    </row>
+    <row r="285" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A285" s="2"/>
       <c r="B285" s="2"/>
       <c r="C285" s="2"/>
@@ -39357,8 +39679,9 @@
       <c r="BE285" s="2"/>
       <c r="BF285" s="2"/>
       <c r="BG285" s="2"/>
-    </row>
-    <row r="286" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="BH285" s="2"/>
+    </row>
+    <row r="286" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A286" s="2"/>
       <c r="B286" s="2"/>
       <c r="C286" s="2"/>
@@ -39417,8 +39740,9 @@
       <c r="BE286" s="2"/>
       <c r="BF286" s="2"/>
       <c r="BG286" s="2"/>
-    </row>
-    <row r="287" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="BH286" s="2"/>
+    </row>
+    <row r="287" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A287" s="2"/>
       <c r="B287" s="2"/>
       <c r="C287" s="2"/>
@@ -39477,8 +39801,9 @@
       <c r="BE287" s="2"/>
       <c r="BF287" s="2"/>
       <c r="BG287" s="2"/>
-    </row>
-    <row r="288" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="BH287" s="2"/>
+    </row>
+    <row r="288" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A288" s="2"/>
       <c r="B288" s="2"/>
       <c r="C288" s="2"/>
@@ -39537,8 +39862,9 @@
       <c r="BE288" s="2"/>
       <c r="BF288" s="2"/>
       <c r="BG288" s="2"/>
-    </row>
-    <row r="289" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="BH288" s="2"/>
+    </row>
+    <row r="289" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A289" s="2"/>
       <c r="B289" s="2"/>
       <c r="C289" s="2"/>
@@ -39597,8 +39923,9 @@
       <c r="BE289" s="2"/>
       <c r="BF289" s="2"/>
       <c r="BG289" s="2"/>
-    </row>
-    <row r="290" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="BH289" s="2"/>
+    </row>
+    <row r="290" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A290" s="2"/>
       <c r="B290" s="2"/>
       <c r="C290" s="2"/>
@@ -39657,8 +39984,9 @@
       <c r="BE290" s="2"/>
       <c r="BF290" s="2"/>
       <c r="BG290" s="2"/>
-    </row>
-    <row r="291" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="BH290" s="2"/>
+    </row>
+    <row r="291" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A291" s="2"/>
       <c r="B291" s="2"/>
       <c r="C291" s="2"/>
@@ -39717,8 +40045,9 @@
       <c r="BE291" s="2"/>
       <c r="BF291" s="2"/>
       <c r="BG291" s="2"/>
-    </row>
-    <row r="292" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="BH291" s="2"/>
+    </row>
+    <row r="292" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A292" s="2"/>
       <c r="B292" s="2"/>
       <c r="C292" s="2"/>
@@ -39741,7 +40070,7 @@
       <c r="U292" s="2"/>
       <c r="V292" s="2"/>
       <c r="W292" s="2"/>
-      <c r="Y292" s="2"/>
+      <c r="X292" s="2"/>
       <c r="Z292" s="2"/>
       <c r="AA292" s="2"/>
       <c r="AB292" s="2"/>
@@ -39776,8 +40105,9 @@
       <c r="BE292" s="2"/>
       <c r="BF292" s="2"/>
       <c r="BG292" s="2"/>
-    </row>
-    <row r="293" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="BH292" s="2"/>
+    </row>
+    <row r="293" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A293" s="2"/>
       <c r="B293" s="2"/>
       <c r="C293" s="2"/>
@@ -39800,7 +40130,7 @@
       <c r="U293" s="2"/>
       <c r="V293" s="2"/>
       <c r="W293" s="2"/>
-      <c r="Y293" s="2"/>
+      <c r="X293" s="2"/>
       <c r="Z293" s="2"/>
       <c r="AA293" s="2"/>
       <c r="AB293" s="2"/>
@@ -39835,8 +40165,9 @@
       <c r="BE293" s="2"/>
       <c r="BF293" s="2"/>
       <c r="BG293" s="2"/>
-    </row>
-    <row r="294" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="BH293" s="2"/>
+    </row>
+    <row r="294" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A294" s="2"/>
       <c r="B294" s="2"/>
       <c r="C294" s="2"/>
@@ -39859,7 +40190,7 @@
       <c r="U294" s="2"/>
       <c r="V294" s="2"/>
       <c r="W294" s="2"/>
-      <c r="Y294" s="2"/>
+      <c r="X294" s="2"/>
       <c r="Z294" s="2"/>
       <c r="AA294" s="2"/>
       <c r="AB294" s="2"/>
@@ -39894,8 +40225,9 @@
       <c r="BE294" s="2"/>
       <c r="BF294" s="2"/>
       <c r="BG294" s="2"/>
-    </row>
-    <row r="295" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="BH294" s="2"/>
+    </row>
+    <row r="295" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A295" s="2"/>
       <c r="B295" s="2"/>
       <c r="C295" s="2"/>
@@ -39917,7 +40249,7 @@
       <c r="T295" s="2"/>
       <c r="U295" s="2"/>
       <c r="V295" s="2"/>
-      <c r="Y295" s="2"/>
+      <c r="W295" s="2"/>
       <c r="Z295" s="2"/>
       <c r="AA295" s="2"/>
       <c r="AB295" s="2"/>
@@ -39952,9 +40284,9 @@
       <c r="BE295" s="2"/>
       <c r="BF295" s="2"/>
       <c r="BG295" s="2"/>
-    </row>
-    <row r="296" spans="1:59" x14ac:dyDescent="0.25">
-      <c r="Y296" s="2"/>
+      <c r="BH295" s="2"/>
+    </row>
+    <row r="296" spans="1:60" x14ac:dyDescent="0.25">
       <c r="Z296" s="2"/>
       <c r="AA296" s="2"/>
       <c r="AB296" s="2"/>
@@ -39989,9 +40321,9 @@
       <c r="BE296" s="2"/>
       <c r="BF296" s="2"/>
       <c r="BG296" s="2"/>
-    </row>
-    <row r="297" spans="1:59" x14ac:dyDescent="0.25">
-      <c r="Y297" s="2"/>
+      <c r="BH296" s="2"/>
+    </row>
+    <row r="297" spans="1:60" x14ac:dyDescent="0.25">
       <c r="Z297" s="2"/>
       <c r="AA297" s="2"/>
       <c r="AB297" s="2"/>
@@ -40026,9 +40358,10 @@
       <c r="BE297" s="2"/>
       <c r="BF297" s="2"/>
       <c r="BG297" s="2"/>
-    </row>
-    <row r="298" spans="1:59" x14ac:dyDescent="0.25">
-      <c r="Y298" s="2"/>
+      <c r="BH297" s="2"/>
+    </row>
+    <row r="298" spans="1:60" x14ac:dyDescent="0.25">
+      <c r="Z298" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>